<commit_message>
change on interactive plotly figure
</commit_message>
<xml_diff>
--- a/data/00_von-bertalanffy-literature.xlsx
+++ b/data/00_von-bertalanffy-literature.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="258">
   <si>
     <t>Family</t>
   </si>
@@ -770,6 +770,30 @@
   </si>
   <si>
     <t>Calotomus</t>
+  </si>
+  <si>
+    <t>Funafuti Atoll, Tuvalu</t>
+  </si>
+  <si>
+    <t>Moore et al, 2013a</t>
+  </si>
+  <si>
+    <t>Moore et al, 2013b</t>
+  </si>
+  <si>
+    <t>Majuro Atoll, Marshall Islands</t>
+  </si>
+  <si>
+    <t>Moore et al, 2015a</t>
+  </si>
+  <si>
+    <t>Andra Island, Papua New Guinea</t>
+  </si>
+  <si>
+    <t>Moore et al, 2015b</t>
+  </si>
+  <si>
+    <t>Pohnpei, Federated States of Micronesia</t>
   </si>
 </sst>
 </file>
@@ -1577,10 +1601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O172"/>
+  <dimension ref="A1:O203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,7 +1613,7 @@
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -9082,6 +9106,1463 @@
       </c>
       <c r="O172" t="s">
         <v>180</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>186</v>
+      </c>
+      <c r="B173" t="s">
+        <v>187</v>
+      </c>
+      <c r="C173" t="s">
+        <v>190</v>
+      </c>
+      <c r="D173">
+        <v>11</v>
+      </c>
+      <c r="E173">
+        <v>0.77</v>
+      </c>
+      <c r="F173">
+        <v>0</v>
+      </c>
+      <c r="G173">
+        <v>17</v>
+      </c>
+      <c r="H173">
+        <v>11</v>
+      </c>
+      <c r="I173">
+        <v>11.7</v>
+      </c>
+      <c r="J173" t="s">
+        <v>36</v>
+      </c>
+      <c r="K173" t="s">
+        <v>45</v>
+      </c>
+      <c r="L173" t="s">
+        <v>90</v>
+      </c>
+      <c r="M173" t="s">
+        <v>250</v>
+      </c>
+      <c r="N173" t="s">
+        <v>251</v>
+      </c>
+      <c r="O173" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>125</v>
+      </c>
+      <c r="B174" t="s">
+        <v>130</v>
+      </c>
+      <c r="C174" t="s">
+        <v>245</v>
+      </c>
+      <c r="D174">
+        <v>47.38</v>
+      </c>
+      <c r="E174">
+        <v>0.41</v>
+      </c>
+      <c r="F174">
+        <v>0</v>
+      </c>
+      <c r="G174">
+        <v>20</v>
+      </c>
+      <c r="H174">
+        <v>11</v>
+      </c>
+      <c r="I174">
+        <v>45.8</v>
+      </c>
+      <c r="J174" t="s">
+        <v>36</v>
+      </c>
+      <c r="K174" t="s">
+        <v>11</v>
+      </c>
+      <c r="L174" t="s">
+        <v>90</v>
+      </c>
+      <c r="M174" t="s">
+        <v>250</v>
+      </c>
+      <c r="N174" t="s">
+        <v>251</v>
+      </c>
+      <c r="O174" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>8</v>
+      </c>
+      <c r="B175" t="s">
+        <v>47</v>
+      </c>
+      <c r="C175" t="s">
+        <v>46</v>
+      </c>
+      <c r="D175">
+        <v>16.920000000000002</v>
+      </c>
+      <c r="E175">
+        <v>0.63</v>
+      </c>
+      <c r="F175">
+        <v>0</v>
+      </c>
+      <c r="G175">
+        <v>41</v>
+      </c>
+      <c r="H175">
+        <v>19</v>
+      </c>
+      <c r="I175">
+        <v>20.2</v>
+      </c>
+      <c r="J175" t="s">
+        <v>36</v>
+      </c>
+      <c r="K175" t="s">
+        <v>45</v>
+      </c>
+      <c r="L175" t="s">
+        <v>90</v>
+      </c>
+      <c r="M175" t="s">
+        <v>250</v>
+      </c>
+      <c r="N175" t="s">
+        <v>251</v>
+      </c>
+      <c r="O175" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>44</v>
+      </c>
+      <c r="B176" t="s">
+        <v>43</v>
+      </c>
+      <c r="C176" t="s">
+        <v>42</v>
+      </c>
+      <c r="D176">
+        <v>16.46</v>
+      </c>
+      <c r="E176">
+        <v>1.01</v>
+      </c>
+      <c r="F176">
+        <v>0</v>
+      </c>
+      <c r="G176">
+        <v>47</v>
+      </c>
+      <c r="H176">
+        <v>6</v>
+      </c>
+      <c r="I176">
+        <v>20.8</v>
+      </c>
+      <c r="J176" t="s">
+        <v>36</v>
+      </c>
+      <c r="K176" t="s">
+        <v>45</v>
+      </c>
+      <c r="L176" t="s">
+        <v>90</v>
+      </c>
+      <c r="M176" t="s">
+        <v>250</v>
+      </c>
+      <c r="N176" t="s">
+        <v>251</v>
+      </c>
+      <c r="O176" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>19</v>
+      </c>
+      <c r="B177" t="s">
+        <v>17</v>
+      </c>
+      <c r="C177" t="s">
+        <v>39</v>
+      </c>
+      <c r="D177">
+        <v>34</v>
+      </c>
+      <c r="E177">
+        <v>0.38</v>
+      </c>
+      <c r="F177">
+        <v>0</v>
+      </c>
+      <c r="G177">
+        <v>49</v>
+      </c>
+      <c r="H177">
+        <v>21</v>
+      </c>
+      <c r="I177">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="J177" t="s">
+        <v>36</v>
+      </c>
+      <c r="K177" t="s">
+        <v>11</v>
+      </c>
+      <c r="L177" t="s">
+        <v>93</v>
+      </c>
+      <c r="M177" t="s">
+        <v>250</v>
+      </c>
+      <c r="N177" t="s">
+        <v>251</v>
+      </c>
+      <c r="O177" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>19</v>
+      </c>
+      <c r="B178" t="s">
+        <v>17</v>
+      </c>
+      <c r="C178" t="s">
+        <v>39</v>
+      </c>
+      <c r="D178">
+        <v>29.35</v>
+      </c>
+      <c r="E178">
+        <v>0.44</v>
+      </c>
+      <c r="F178">
+        <v>0</v>
+      </c>
+      <c r="G178">
+        <v>49</v>
+      </c>
+      <c r="H178">
+        <v>21</v>
+      </c>
+      <c r="I178">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="J178" t="s">
+        <v>36</v>
+      </c>
+      <c r="K178" t="s">
+        <v>11</v>
+      </c>
+      <c r="L178" t="s">
+        <v>94</v>
+      </c>
+      <c r="M178" t="s">
+        <v>250</v>
+      </c>
+      <c r="N178" t="s">
+        <v>251</v>
+      </c>
+      <c r="O178" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>19</v>
+      </c>
+      <c r="B179" t="s">
+        <v>17</v>
+      </c>
+      <c r="C179" t="s">
+        <v>153</v>
+      </c>
+      <c r="D179">
+        <v>22.37</v>
+      </c>
+      <c r="E179">
+        <v>0.6</v>
+      </c>
+      <c r="F179">
+        <v>0</v>
+      </c>
+      <c r="G179">
+        <v>43</v>
+      </c>
+      <c r="H179">
+        <v>6</v>
+      </c>
+      <c r="I179">
+        <v>23.4</v>
+      </c>
+      <c r="J179" t="s">
+        <v>36</v>
+      </c>
+      <c r="K179" t="s">
+        <v>11</v>
+      </c>
+      <c r="L179" t="s">
+        <v>93</v>
+      </c>
+      <c r="M179" t="s">
+        <v>250</v>
+      </c>
+      <c r="N179" t="s">
+        <v>251</v>
+      </c>
+      <c r="O179" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>19</v>
+      </c>
+      <c r="B180" t="s">
+        <v>17</v>
+      </c>
+      <c r="C180" t="s">
+        <v>153</v>
+      </c>
+      <c r="D180">
+        <v>19.75</v>
+      </c>
+      <c r="E180">
+        <v>0.91</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+      <c r="G180">
+        <v>43</v>
+      </c>
+      <c r="H180">
+        <v>6</v>
+      </c>
+      <c r="I180">
+        <v>23.4</v>
+      </c>
+      <c r="J180" t="s">
+        <v>36</v>
+      </c>
+      <c r="K180" t="s">
+        <v>11</v>
+      </c>
+      <c r="L180" t="s">
+        <v>94</v>
+      </c>
+      <c r="M180" t="s">
+        <v>250</v>
+      </c>
+      <c r="N180" t="s">
+        <v>251</v>
+      </c>
+      <c r="O180" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>8</v>
+      </c>
+      <c r="B181" t="s">
+        <v>9</v>
+      </c>
+      <c r="C181" t="s">
+        <v>65</v>
+      </c>
+      <c r="D181">
+        <v>27.05</v>
+      </c>
+      <c r="E181">
+        <v>0.92</v>
+      </c>
+      <c r="F181">
+        <v>0</v>
+      </c>
+      <c r="G181">
+        <v>39</v>
+      </c>
+      <c r="H181">
+        <v>20</v>
+      </c>
+      <c r="I181">
+        <v>30.1</v>
+      </c>
+      <c r="J181" t="s">
+        <v>36</v>
+      </c>
+      <c r="K181" t="s">
+        <v>11</v>
+      </c>
+      <c r="L181" t="s">
+        <v>93</v>
+      </c>
+      <c r="M181" t="s">
+        <v>250</v>
+      </c>
+      <c r="N181" t="s">
+        <v>251</v>
+      </c>
+      <c r="O181" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>8</v>
+      </c>
+      <c r="B182" t="s">
+        <v>9</v>
+      </c>
+      <c r="C182" t="s">
+        <v>65</v>
+      </c>
+      <c r="D182">
+        <v>23.22</v>
+      </c>
+      <c r="E182">
+        <v>1.05</v>
+      </c>
+      <c r="F182">
+        <v>0</v>
+      </c>
+      <c r="G182">
+        <v>39</v>
+      </c>
+      <c r="H182">
+        <v>20</v>
+      </c>
+      <c r="I182">
+        <v>30.1</v>
+      </c>
+      <c r="J182" t="s">
+        <v>36</v>
+      </c>
+      <c r="K182" t="s">
+        <v>11</v>
+      </c>
+      <c r="L182" t="s">
+        <v>94</v>
+      </c>
+      <c r="M182" t="s">
+        <v>250</v>
+      </c>
+      <c r="N182" t="s">
+        <v>251</v>
+      </c>
+      <c r="O182" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>186</v>
+      </c>
+      <c r="B183" t="s">
+        <v>187</v>
+      </c>
+      <c r="C183" t="s">
+        <v>190</v>
+      </c>
+      <c r="D183">
+        <v>10.99</v>
+      </c>
+      <c r="E183">
+        <v>1.82</v>
+      </c>
+      <c r="F183">
+        <v>0</v>
+      </c>
+      <c r="G183">
+        <v>30</v>
+      </c>
+      <c r="H183">
+        <v>4</v>
+      </c>
+      <c r="I183">
+        <v>11.7</v>
+      </c>
+      <c r="J183" t="s">
+        <v>36</v>
+      </c>
+      <c r="K183" t="s">
+        <v>45</v>
+      </c>
+      <c r="L183" t="s">
+        <v>90</v>
+      </c>
+      <c r="M183" t="s">
+        <v>253</v>
+      </c>
+      <c r="N183" t="s">
+        <v>252</v>
+      </c>
+      <c r="O183" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>8</v>
+      </c>
+      <c r="B184" t="s">
+        <v>47</v>
+      </c>
+      <c r="C184" t="s">
+        <v>46</v>
+      </c>
+      <c r="D184">
+        <v>15.75</v>
+      </c>
+      <c r="E184">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="F184">
+        <v>0</v>
+      </c>
+      <c r="G184">
+        <v>46</v>
+      </c>
+      <c r="H184">
+        <v>17</v>
+      </c>
+      <c r="I184">
+        <v>19.5</v>
+      </c>
+      <c r="J184" t="s">
+        <v>36</v>
+      </c>
+      <c r="K184" t="s">
+        <v>11</v>
+      </c>
+      <c r="L184" t="s">
+        <v>90</v>
+      </c>
+      <c r="M184" t="s">
+        <v>253</v>
+      </c>
+      <c r="N184" t="s">
+        <v>252</v>
+      </c>
+      <c r="O184" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>19</v>
+      </c>
+      <c r="B185" t="s">
+        <v>17</v>
+      </c>
+      <c r="C185" t="s">
+        <v>39</v>
+      </c>
+      <c r="D185">
+        <v>28.47</v>
+      </c>
+      <c r="E185">
+        <v>0.53</v>
+      </c>
+      <c r="F185">
+        <v>0</v>
+      </c>
+      <c r="G185">
+        <v>52</v>
+      </c>
+      <c r="H185">
+        <v>21</v>
+      </c>
+      <c r="I185">
+        <v>32.6</v>
+      </c>
+      <c r="J185" t="s">
+        <v>36</v>
+      </c>
+      <c r="K185" t="s">
+        <v>11</v>
+      </c>
+      <c r="L185" t="s">
+        <v>93</v>
+      </c>
+      <c r="M185" t="s">
+        <v>253</v>
+      </c>
+      <c r="N185" t="s">
+        <v>252</v>
+      </c>
+      <c r="O185" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>19</v>
+      </c>
+      <c r="B186" t="s">
+        <v>17</v>
+      </c>
+      <c r="C186" t="s">
+        <v>39</v>
+      </c>
+      <c r="D186">
+        <v>26.5</v>
+      </c>
+      <c r="E186">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F186">
+        <v>0</v>
+      </c>
+      <c r="G186">
+        <v>52</v>
+      </c>
+      <c r="H186">
+        <v>21</v>
+      </c>
+      <c r="I186">
+        <v>32.6</v>
+      </c>
+      <c r="J186" t="s">
+        <v>36</v>
+      </c>
+      <c r="K186" t="s">
+        <v>11</v>
+      </c>
+      <c r="L186" t="s">
+        <v>94</v>
+      </c>
+      <c r="M186" t="s">
+        <v>253</v>
+      </c>
+      <c r="N186" t="s">
+        <v>252</v>
+      </c>
+      <c r="O186" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>8</v>
+      </c>
+      <c r="B187" t="s">
+        <v>9</v>
+      </c>
+      <c r="C187" t="s">
+        <v>65</v>
+      </c>
+      <c r="D187">
+        <v>26.59</v>
+      </c>
+      <c r="E187">
+        <v>0.79</v>
+      </c>
+      <c r="F187">
+        <v>0</v>
+      </c>
+      <c r="G187">
+        <v>52</v>
+      </c>
+      <c r="H187">
+        <v>20</v>
+      </c>
+      <c r="I187">
+        <v>28.1</v>
+      </c>
+      <c r="J187" t="s">
+        <v>36</v>
+      </c>
+      <c r="K187" t="s">
+        <v>11</v>
+      </c>
+      <c r="L187" t="s">
+        <v>93</v>
+      </c>
+      <c r="M187" t="s">
+        <v>253</v>
+      </c>
+      <c r="N187" t="s">
+        <v>252</v>
+      </c>
+      <c r="O187" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>8</v>
+      </c>
+      <c r="B188" t="s">
+        <v>9</v>
+      </c>
+      <c r="C188" t="s">
+        <v>65</v>
+      </c>
+      <c r="D188">
+        <v>23.43</v>
+      </c>
+      <c r="E188">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F188">
+        <v>0</v>
+      </c>
+      <c r="G188">
+        <v>52</v>
+      </c>
+      <c r="H188">
+        <v>20</v>
+      </c>
+      <c r="I188">
+        <v>28.1</v>
+      </c>
+      <c r="J188" t="s">
+        <v>36</v>
+      </c>
+      <c r="K188" t="s">
+        <v>11</v>
+      </c>
+      <c r="L188" t="s">
+        <v>94</v>
+      </c>
+      <c r="M188" t="s">
+        <v>253</v>
+      </c>
+      <c r="N188" t="s">
+        <v>252</v>
+      </c>
+      <c r="O188" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>186</v>
+      </c>
+      <c r="B189" t="s">
+        <v>187</v>
+      </c>
+      <c r="C189" t="s">
+        <v>190</v>
+      </c>
+      <c r="D189">
+        <v>10.7</v>
+      </c>
+      <c r="E189">
+        <v>1.01</v>
+      </c>
+      <c r="F189">
+        <v>0</v>
+      </c>
+      <c r="G189">
+        <v>44</v>
+      </c>
+      <c r="H189">
+        <v>9</v>
+      </c>
+      <c r="I189">
+        <v>11.4</v>
+      </c>
+      <c r="J189" t="s">
+        <v>36</v>
+      </c>
+      <c r="K189" t="s">
+        <v>45</v>
+      </c>
+      <c r="L189" t="s">
+        <v>90</v>
+      </c>
+      <c r="M189" t="s">
+        <v>255</v>
+      </c>
+      <c r="N189" t="s">
+        <v>254</v>
+      </c>
+      <c r="O189" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>8</v>
+      </c>
+      <c r="B190" t="s">
+        <v>47</v>
+      </c>
+      <c r="C190" t="s">
+        <v>46</v>
+      </c>
+      <c r="D190">
+        <v>16.8</v>
+      </c>
+      <c r="E190">
+        <v>0.98</v>
+      </c>
+      <c r="F190">
+        <v>0</v>
+      </c>
+      <c r="G190">
+        <v>42</v>
+      </c>
+      <c r="H190">
+        <v>6</v>
+      </c>
+      <c r="I190">
+        <v>18.8</v>
+      </c>
+      <c r="J190" t="s">
+        <v>36</v>
+      </c>
+      <c r="K190" t="s">
+        <v>11</v>
+      </c>
+      <c r="L190" t="s">
+        <v>90</v>
+      </c>
+      <c r="M190" t="s">
+        <v>255</v>
+      </c>
+      <c r="N190" t="s">
+        <v>254</v>
+      </c>
+      <c r="O190" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>19</v>
+      </c>
+      <c r="B191" t="s">
+        <v>17</v>
+      </c>
+      <c r="C191" t="s">
+        <v>39</v>
+      </c>
+      <c r="D191">
+        <v>30.5</v>
+      </c>
+      <c r="E191">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F191">
+        <v>0</v>
+      </c>
+      <c r="G191">
+        <v>45</v>
+      </c>
+      <c r="H191">
+        <v>11</v>
+      </c>
+      <c r="I191">
+        <v>31.2</v>
+      </c>
+      <c r="J191" t="s">
+        <v>36</v>
+      </c>
+      <c r="K191" t="s">
+        <v>11</v>
+      </c>
+      <c r="L191" t="s">
+        <v>93</v>
+      </c>
+      <c r="M191" t="s">
+        <v>255</v>
+      </c>
+      <c r="N191" t="s">
+        <v>254</v>
+      </c>
+      <c r="O191" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>19</v>
+      </c>
+      <c r="B192" t="s">
+        <v>17</v>
+      </c>
+      <c r="C192" t="s">
+        <v>39</v>
+      </c>
+      <c r="D192">
+        <v>26.7</v>
+      </c>
+      <c r="E192">
+        <v>0.83</v>
+      </c>
+      <c r="F192">
+        <v>0</v>
+      </c>
+      <c r="G192">
+        <v>45</v>
+      </c>
+      <c r="H192">
+        <v>11</v>
+      </c>
+      <c r="I192">
+        <v>31.2</v>
+      </c>
+      <c r="J192" t="s">
+        <v>36</v>
+      </c>
+      <c r="K192" t="s">
+        <v>11</v>
+      </c>
+      <c r="L192" t="s">
+        <v>94</v>
+      </c>
+      <c r="M192" t="s">
+        <v>255</v>
+      </c>
+      <c r="N192" t="s">
+        <v>254</v>
+      </c>
+      <c r="O192" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>8</v>
+      </c>
+      <c r="B193" t="s">
+        <v>9</v>
+      </c>
+      <c r="C193" t="s">
+        <v>65</v>
+      </c>
+      <c r="D193">
+        <v>23.2</v>
+      </c>
+      <c r="E193">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F193">
+        <v>0</v>
+      </c>
+      <c r="G193">
+        <v>41</v>
+      </c>
+      <c r="H193">
+        <v>17</v>
+      </c>
+      <c r="I193">
+        <v>23.6</v>
+      </c>
+      <c r="J193" t="s">
+        <v>36</v>
+      </c>
+      <c r="K193" t="s">
+        <v>11</v>
+      </c>
+      <c r="L193" t="s">
+        <v>93</v>
+      </c>
+      <c r="M193" t="s">
+        <v>255</v>
+      </c>
+      <c r="N193" t="s">
+        <v>254</v>
+      </c>
+      <c r="O193" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>8</v>
+      </c>
+      <c r="B194" t="s">
+        <v>9</v>
+      </c>
+      <c r="C194" t="s">
+        <v>65</v>
+      </c>
+      <c r="D194">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E194">
+        <v>1.92</v>
+      </c>
+      <c r="F194">
+        <v>0</v>
+      </c>
+      <c r="G194">
+        <v>41</v>
+      </c>
+      <c r="H194">
+        <v>17</v>
+      </c>
+      <c r="I194">
+        <v>23.6</v>
+      </c>
+      <c r="J194" t="s">
+        <v>36</v>
+      </c>
+      <c r="K194" t="s">
+        <v>11</v>
+      </c>
+      <c r="L194" t="s">
+        <v>94</v>
+      </c>
+      <c r="M194" t="s">
+        <v>255</v>
+      </c>
+      <c r="N194" t="s">
+        <v>254</v>
+      </c>
+      <c r="O194" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>44</v>
+      </c>
+      <c r="B195" t="s">
+        <v>76</v>
+      </c>
+      <c r="C195" t="s">
+        <v>98</v>
+      </c>
+      <c r="D195">
+        <v>31.44</v>
+      </c>
+      <c r="E195">
+        <v>0.255</v>
+      </c>
+      <c r="F195">
+        <v>0</v>
+      </c>
+      <c r="G195">
+        <v>31</v>
+      </c>
+      <c r="H195">
+        <v>15</v>
+      </c>
+      <c r="I195">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="J195" t="s">
+        <v>36</v>
+      </c>
+      <c r="K195" t="s">
+        <v>45</v>
+      </c>
+      <c r="L195" t="s">
+        <v>90</v>
+      </c>
+      <c r="M195" t="s">
+        <v>257</v>
+      </c>
+      <c r="N195" t="s">
+        <v>256</v>
+      </c>
+      <c r="O195" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>186</v>
+      </c>
+      <c r="B196" t="s">
+        <v>187</v>
+      </c>
+      <c r="C196" t="s">
+        <v>190</v>
+      </c>
+      <c r="D196">
+        <v>10.52</v>
+      </c>
+      <c r="E196">
+        <v>1.91</v>
+      </c>
+      <c r="F196">
+        <v>0</v>
+      </c>
+      <c r="G196">
+        <v>39</v>
+      </c>
+      <c r="H196">
+        <v>9</v>
+      </c>
+      <c r="I196">
+        <v>11.5</v>
+      </c>
+      <c r="J196" t="s">
+        <v>36</v>
+      </c>
+      <c r="K196" t="s">
+        <v>45</v>
+      </c>
+      <c r="L196" t="s">
+        <v>90</v>
+      </c>
+      <c r="M196" t="s">
+        <v>257</v>
+      </c>
+      <c r="N196" t="s">
+        <v>256</v>
+      </c>
+      <c r="O196" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>8</v>
+      </c>
+      <c r="B197" t="s">
+        <v>47</v>
+      </c>
+      <c r="C197" t="s">
+        <v>46</v>
+      </c>
+      <c r="D197">
+        <v>15.05</v>
+      </c>
+      <c r="E197">
+        <v>1.3180000000000001</v>
+      </c>
+      <c r="F197">
+        <v>0</v>
+      </c>
+      <c r="G197">
+        <v>55</v>
+      </c>
+      <c r="H197">
+        <v>11</v>
+      </c>
+      <c r="I197">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="J197" t="s">
+        <v>36</v>
+      </c>
+      <c r="K197" t="s">
+        <v>11</v>
+      </c>
+      <c r="L197" t="s">
+        <v>90</v>
+      </c>
+      <c r="M197" t="s">
+        <v>257</v>
+      </c>
+      <c r="N197" t="s">
+        <v>256</v>
+      </c>
+      <c r="O197" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>19</v>
+      </c>
+      <c r="B198" t="s">
+        <v>17</v>
+      </c>
+      <c r="C198" t="s">
+        <v>18</v>
+      </c>
+      <c r="D198">
+        <v>20.34</v>
+      </c>
+      <c r="E198">
+        <v>1.306</v>
+      </c>
+      <c r="F198">
+        <v>0</v>
+      </c>
+      <c r="G198">
+        <v>78</v>
+      </c>
+      <c r="H198">
+        <v>19</v>
+      </c>
+      <c r="I198">
+        <v>28.7</v>
+      </c>
+      <c r="J198" t="s">
+        <v>36</v>
+      </c>
+      <c r="K198" t="s">
+        <v>11</v>
+      </c>
+      <c r="L198" t="s">
+        <v>93</v>
+      </c>
+      <c r="M198" t="s">
+        <v>257</v>
+      </c>
+      <c r="N198" t="s">
+        <v>256</v>
+      </c>
+      <c r="O198" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>19</v>
+      </c>
+      <c r="B199" t="s">
+        <v>17</v>
+      </c>
+      <c r="C199" t="s">
+        <v>18</v>
+      </c>
+      <c r="D199">
+        <v>23.62</v>
+      </c>
+      <c r="E199">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="F199">
+        <v>0</v>
+      </c>
+      <c r="G199">
+        <v>78</v>
+      </c>
+      <c r="H199">
+        <v>19</v>
+      </c>
+      <c r="I199">
+        <v>28.7</v>
+      </c>
+      <c r="J199" t="s">
+        <v>36</v>
+      </c>
+      <c r="K199" t="s">
+        <v>11</v>
+      </c>
+      <c r="L199" t="s">
+        <v>94</v>
+      </c>
+      <c r="M199" t="s">
+        <v>257</v>
+      </c>
+      <c r="N199" t="s">
+        <v>256</v>
+      </c>
+      <c r="O199" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>19</v>
+      </c>
+      <c r="B200" t="s">
+        <v>17</v>
+      </c>
+      <c r="C200" t="s">
+        <v>39</v>
+      </c>
+      <c r="D200">
+        <v>32.479999999999997</v>
+      </c>
+      <c r="E200">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="F200">
+        <v>0</v>
+      </c>
+      <c r="G200">
+        <v>90</v>
+      </c>
+      <c r="H200">
+        <v>16</v>
+      </c>
+      <c r="I200">
+        <v>36.4</v>
+      </c>
+      <c r="J200" t="s">
+        <v>36</v>
+      </c>
+      <c r="K200" t="s">
+        <v>11</v>
+      </c>
+      <c r="L200" t="s">
+        <v>93</v>
+      </c>
+      <c r="M200" t="s">
+        <v>257</v>
+      </c>
+      <c r="N200" t="s">
+        <v>256</v>
+      </c>
+      <c r="O200" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>19</v>
+      </c>
+      <c r="B201" t="s">
+        <v>17</v>
+      </c>
+      <c r="C201" t="s">
+        <v>39</v>
+      </c>
+      <c r="D201">
+        <v>26.67</v>
+      </c>
+      <c r="E201">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="F201">
+        <v>0</v>
+      </c>
+      <c r="G201">
+        <v>90</v>
+      </c>
+      <c r="H201">
+        <v>16</v>
+      </c>
+      <c r="I201">
+        <v>36.4</v>
+      </c>
+      <c r="J201" t="s">
+        <v>36</v>
+      </c>
+      <c r="K201" t="s">
+        <v>11</v>
+      </c>
+      <c r="L201" t="s">
+        <v>94</v>
+      </c>
+      <c r="M201" t="s">
+        <v>257</v>
+      </c>
+      <c r="N201" t="s">
+        <v>256</v>
+      </c>
+      <c r="O201" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>8</v>
+      </c>
+      <c r="B202" t="s">
+        <v>9</v>
+      </c>
+      <c r="C202" t="s">
+        <v>65</v>
+      </c>
+      <c r="D202">
+        <v>23.77</v>
+      </c>
+      <c r="E202">
+        <v>1.171</v>
+      </c>
+      <c r="F202">
+        <v>0</v>
+      </c>
+      <c r="G202">
+        <v>71</v>
+      </c>
+      <c r="H202">
+        <v>13</v>
+      </c>
+      <c r="I202">
+        <v>25</v>
+      </c>
+      <c r="J202" t="s">
+        <v>36</v>
+      </c>
+      <c r="K202" t="s">
+        <v>11</v>
+      </c>
+      <c r="L202" t="s">
+        <v>93</v>
+      </c>
+      <c r="M202" t="s">
+        <v>257</v>
+      </c>
+      <c r="N202" t="s">
+        <v>256</v>
+      </c>
+      <c r="O202" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>8</v>
+      </c>
+      <c r="B203" t="s">
+        <v>9</v>
+      </c>
+      <c r="C203" t="s">
+        <v>65</v>
+      </c>
+      <c r="D203">
+        <v>20.72</v>
+      </c>
+      <c r="E203">
+        <v>2.0550000000000002</v>
+      </c>
+      <c r="F203">
+        <v>0</v>
+      </c>
+      <c r="G203">
+        <v>71</v>
+      </c>
+      <c r="H203">
+        <v>13</v>
+      </c>
+      <c r="I203">
+        <v>25</v>
+      </c>
+      <c r="J203" t="s">
+        <v>36</v>
+      </c>
+      <c r="K203" t="s">
+        <v>11</v>
+      </c>
+      <c r="L203" t="s">
+        <v>94</v>
+      </c>
+      <c r="M203" t="s">
+        <v>257</v>
+      </c>
+      <c r="N203" t="s">
+        <v>256</v>
+      </c>
+      <c r="O203" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change parameters for non convergent models
</commit_message>
<xml_diff>
--- a/data/00_von-bertalanffy-literature.xlsx
+++ b/data/00_von-bertalanffy-literature.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="257">
   <si>
     <t>Family</t>
   </si>
@@ -413,9 +413,6 @@
   </si>
   <si>
     <t>Chlorurus</t>
-  </si>
-  <si>
-    <t>Chlorurus microrbinos</t>
   </si>
   <si>
     <t>Chlorurus sordidus</t>
@@ -1603,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O203"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,7 +1659,7 @@
         <v>7</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1709,7 +1706,7 @@
         <v>12</v>
       </c>
       <c r="O2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1756,7 +1753,7 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1803,7 +1800,7 @@
         <v>37</v>
       </c>
       <c r="O4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1850,7 +1847,7 @@
         <v>40</v>
       </c>
       <c r="O5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1897,7 +1894,7 @@
         <v>48</v>
       </c>
       <c r="O6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1944,7 +1941,7 @@
         <v>48</v>
       </c>
       <c r="O7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1991,7 +1988,7 @@
         <v>48</v>
       </c>
       <c r="O8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2038,7 +2035,7 @@
         <v>48</v>
       </c>
       <c r="O9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2085,7 +2082,7 @@
         <v>48</v>
       </c>
       <c r="O10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2132,7 +2129,7 @@
         <v>48</v>
       </c>
       <c r="O11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -2179,7 +2176,7 @@
         <v>48</v>
       </c>
       <c r="O12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2226,7 +2223,7 @@
         <v>48</v>
       </c>
       <c r="O13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2273,7 +2270,7 @@
         <v>48</v>
       </c>
       <c r="O14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2320,7 +2317,7 @@
         <v>48</v>
       </c>
       <c r="O15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2367,7 +2364,7 @@
         <v>48</v>
       </c>
       <c r="O16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -2414,7 +2411,7 @@
         <v>48</v>
       </c>
       <c r="O17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -2461,7 +2458,7 @@
         <v>48</v>
       </c>
       <c r="O18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -2508,7 +2505,7 @@
         <v>48</v>
       </c>
       <c r="O19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -2555,7 +2552,7 @@
         <v>48</v>
       </c>
       <c r="O20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -2602,7 +2599,7 @@
         <v>64</v>
       </c>
       <c r="O21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2649,7 +2646,7 @@
         <v>64</v>
       </c>
       <c r="O22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -2696,7 +2693,7 @@
         <v>64</v>
       </c>
       <c r="O23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2743,7 +2740,7 @@
         <v>64</v>
       </c>
       <c r="O24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -2787,7 +2784,7 @@
         <v>68</v>
       </c>
       <c r="O25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2834,7 +2831,7 @@
         <v>74</v>
       </c>
       <c r="O26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2875,7 +2872,7 @@
         <v>75</v>
       </c>
       <c r="O27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2916,7 +2913,7 @@
         <v>75</v>
       </c>
       <c r="O28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -2960,7 +2957,7 @@
         <v>81</v>
       </c>
       <c r="O29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -3004,7 +3001,7 @@
         <v>81</v>
       </c>
       <c r="O30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -3048,7 +3045,7 @@
         <v>81</v>
       </c>
       <c r="O31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -3092,7 +3089,7 @@
         <v>81</v>
       </c>
       <c r="O32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -3136,7 +3133,7 @@
         <v>81</v>
       </c>
       <c r="O33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -3180,7 +3177,7 @@
         <v>81</v>
       </c>
       <c r="O34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -3227,7 +3224,7 @@
         <v>92</v>
       </c>
       <c r="O35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -3274,7 +3271,7 @@
         <v>92</v>
       </c>
       <c r="O36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -3321,7 +3318,7 @@
         <v>97</v>
       </c>
       <c r="O37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -3368,7 +3365,7 @@
         <v>100</v>
       </c>
       <c r="O38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -3412,7 +3409,7 @@
         <v>101</v>
       </c>
       <c r="O39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -3456,7 +3453,7 @@
         <v>101</v>
       </c>
       <c r="O40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -3500,7 +3497,7 @@
         <v>101</v>
       </c>
       <c r="O41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -3544,7 +3541,7 @@
         <v>101</v>
       </c>
       <c r="O42" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -3588,7 +3585,7 @@
         <v>101</v>
       </c>
       <c r="O43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -3620,16 +3617,16 @@
         <v>16</v>
       </c>
       <c r="K44" t="s">
+        <v>146</v>
+      </c>
+      <c r="L44" t="s">
+        <v>90</v>
+      </c>
+      <c r="N44" t="s">
         <v>147</v>
       </c>
-      <c r="L44" t="s">
-        <v>90</v>
-      </c>
-      <c r="N44" t="s">
-        <v>148</v>
-      </c>
       <c r="O44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -3661,16 +3658,16 @@
         <v>16</v>
       </c>
       <c r="K45" t="s">
+        <v>146</v>
+      </c>
+      <c r="L45" t="s">
+        <v>90</v>
+      </c>
+      <c r="N45" t="s">
         <v>147</v>
       </c>
-      <c r="L45" t="s">
-        <v>90</v>
-      </c>
-      <c r="N45" t="s">
-        <v>148</v>
-      </c>
       <c r="O45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
@@ -3702,16 +3699,16 @@
         <v>16</v>
       </c>
       <c r="K46" t="s">
+        <v>146</v>
+      </c>
+      <c r="L46" t="s">
+        <v>90</v>
+      </c>
+      <c r="N46" t="s">
         <v>147</v>
       </c>
-      <c r="L46" t="s">
-        <v>90</v>
-      </c>
-      <c r="N46" t="s">
-        <v>148</v>
-      </c>
       <c r="O46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
@@ -3743,16 +3740,16 @@
         <v>16</v>
       </c>
       <c r="K47" t="s">
+        <v>146</v>
+      </c>
+      <c r="L47" t="s">
+        <v>90</v>
+      </c>
+      <c r="N47" t="s">
         <v>147</v>
       </c>
-      <c r="L47" t="s">
-        <v>90</v>
-      </c>
-      <c r="N47" t="s">
-        <v>148</v>
-      </c>
       <c r="O47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
@@ -3784,16 +3781,16 @@
         <v>16</v>
       </c>
       <c r="K48" t="s">
+        <v>146</v>
+      </c>
+      <c r="L48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N48" t="s">
         <v>147</v>
       </c>
-      <c r="L48" t="s">
-        <v>90</v>
-      </c>
-      <c r="N48" t="s">
-        <v>148</v>
-      </c>
       <c r="O48" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -3825,16 +3822,16 @@
         <v>16</v>
       </c>
       <c r="K49" t="s">
+        <v>146</v>
+      </c>
+      <c r="L49" t="s">
+        <v>90</v>
+      </c>
+      <c r="N49" t="s">
         <v>147</v>
       </c>
-      <c r="L49" t="s">
-        <v>90</v>
-      </c>
-      <c r="N49" t="s">
-        <v>148</v>
-      </c>
       <c r="O49" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -3866,16 +3863,16 @@
         <v>16</v>
       </c>
       <c r="K50" t="s">
+        <v>146</v>
+      </c>
+      <c r="L50" t="s">
+        <v>90</v>
+      </c>
+      <c r="N50" t="s">
         <v>147</v>
       </c>
-      <c r="L50" t="s">
-        <v>90</v>
-      </c>
-      <c r="N50" t="s">
-        <v>148</v>
-      </c>
       <c r="O50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -3907,16 +3904,16 @@
         <v>16</v>
       </c>
       <c r="K51" t="s">
+        <v>146</v>
+      </c>
+      <c r="L51" t="s">
+        <v>90</v>
+      </c>
+      <c r="N51" t="s">
         <v>147</v>
       </c>
-      <c r="L51" t="s">
-        <v>90</v>
-      </c>
-      <c r="N51" t="s">
-        <v>148</v>
-      </c>
       <c r="O51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -3948,16 +3945,16 @@
         <v>16</v>
       </c>
       <c r="K52" t="s">
+        <v>146</v>
+      </c>
+      <c r="L52" t="s">
+        <v>90</v>
+      </c>
+      <c r="N52" t="s">
         <v>147</v>
       </c>
-      <c r="L52" t="s">
-        <v>90</v>
-      </c>
-      <c r="N52" t="s">
-        <v>148</v>
-      </c>
       <c r="O52" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -3989,16 +3986,16 @@
         <v>16</v>
       </c>
       <c r="K53" t="s">
+        <v>146</v>
+      </c>
+      <c r="L53" t="s">
+        <v>90</v>
+      </c>
+      <c r="N53" t="s">
         <v>147</v>
       </c>
-      <c r="L53" t="s">
-        <v>90</v>
-      </c>
-      <c r="N53" t="s">
-        <v>148</v>
-      </c>
       <c r="O53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -4030,16 +4027,16 @@
         <v>16</v>
       </c>
       <c r="K54" t="s">
+        <v>146</v>
+      </c>
+      <c r="L54" t="s">
+        <v>90</v>
+      </c>
+      <c r="N54" t="s">
         <v>147</v>
       </c>
-      <c r="L54" t="s">
-        <v>90</v>
-      </c>
-      <c r="N54" t="s">
-        <v>148</v>
-      </c>
       <c r="O54" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -4071,16 +4068,16 @@
         <v>16</v>
       </c>
       <c r="K55" t="s">
+        <v>146</v>
+      </c>
+      <c r="L55" t="s">
+        <v>90</v>
+      </c>
+      <c r="N55" t="s">
         <v>147</v>
       </c>
-      <c r="L55" t="s">
-        <v>90</v>
-      </c>
-      <c r="N55" t="s">
-        <v>148</v>
-      </c>
       <c r="O55" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
@@ -4112,16 +4109,16 @@
         <v>16</v>
       </c>
       <c r="K56" t="s">
+        <v>146</v>
+      </c>
+      <c r="L56" t="s">
+        <v>90</v>
+      </c>
+      <c r="N56" t="s">
         <v>147</v>
       </c>
-      <c r="L56" t="s">
-        <v>90</v>
-      </c>
-      <c r="N56" t="s">
-        <v>148</v>
-      </c>
       <c r="O56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -4153,16 +4150,16 @@
         <v>16</v>
       </c>
       <c r="K57" t="s">
+        <v>146</v>
+      </c>
+      <c r="L57" t="s">
+        <v>90</v>
+      </c>
+      <c r="N57" t="s">
         <v>147</v>
       </c>
-      <c r="L57" t="s">
-        <v>90</v>
-      </c>
-      <c r="N57" t="s">
-        <v>148</v>
-      </c>
       <c r="O57" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
@@ -4194,16 +4191,16 @@
         <v>16</v>
       </c>
       <c r="K58" t="s">
+        <v>146</v>
+      </c>
+      <c r="L58" t="s">
+        <v>90</v>
+      </c>
+      <c r="N58" t="s">
         <v>147</v>
       </c>
-      <c r="L58" t="s">
-        <v>90</v>
-      </c>
-      <c r="N58" t="s">
-        <v>148</v>
-      </c>
       <c r="O58" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
@@ -4235,16 +4232,16 @@
         <v>16</v>
       </c>
       <c r="K59" t="s">
+        <v>146</v>
+      </c>
+      <c r="L59" t="s">
+        <v>90</v>
+      </c>
+      <c r="N59" t="s">
         <v>147</v>
       </c>
-      <c r="L59" t="s">
-        <v>90</v>
-      </c>
-      <c r="N59" t="s">
-        <v>148</v>
-      </c>
       <c r="O59" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
@@ -4276,16 +4273,16 @@
         <v>16</v>
       </c>
       <c r="K60" t="s">
+        <v>146</v>
+      </c>
+      <c r="L60" t="s">
+        <v>90</v>
+      </c>
+      <c r="N60" t="s">
         <v>147</v>
       </c>
-      <c r="L60" t="s">
-        <v>90</v>
-      </c>
-      <c r="N60" t="s">
-        <v>148</v>
-      </c>
       <c r="O60" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
@@ -4317,16 +4314,16 @@
         <v>16</v>
       </c>
       <c r="K61" t="s">
+        <v>146</v>
+      </c>
+      <c r="L61" t="s">
+        <v>90</v>
+      </c>
+      <c r="N61" t="s">
         <v>147</v>
       </c>
-      <c r="L61" t="s">
-        <v>90</v>
-      </c>
-      <c r="N61" t="s">
-        <v>148</v>
-      </c>
       <c r="O61" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
@@ -4358,16 +4355,16 @@
         <v>16</v>
       </c>
       <c r="K62" t="s">
+        <v>146</v>
+      </c>
+      <c r="L62" t="s">
+        <v>90</v>
+      </c>
+      <c r="N62" t="s">
         <v>147</v>
       </c>
-      <c r="L62" t="s">
-        <v>90</v>
-      </c>
-      <c r="N62" t="s">
-        <v>148</v>
-      </c>
       <c r="O62" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
@@ -4378,7 +4375,7 @@
         <v>130</v>
       </c>
       <c r="C63" t="s">
-        <v>131</v>
+        <v>244</v>
       </c>
       <c r="D63">
         <v>429.89</v>
@@ -4399,16 +4396,16 @@
         <v>16</v>
       </c>
       <c r="K63" t="s">
+        <v>146</v>
+      </c>
+      <c r="L63" t="s">
+        <v>90</v>
+      </c>
+      <c r="N63" t="s">
         <v>147</v>
       </c>
-      <c r="L63" t="s">
-        <v>90</v>
-      </c>
-      <c r="N63" t="s">
-        <v>148</v>
-      </c>
       <c r="O63" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
@@ -4419,7 +4416,7 @@
         <v>130</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D64">
         <v>192.95</v>
@@ -4440,16 +4437,16 @@
         <v>16</v>
       </c>
       <c r="K64" t="s">
+        <v>146</v>
+      </c>
+      <c r="L64" t="s">
+        <v>90</v>
+      </c>
+      <c r="N64" t="s">
         <v>147</v>
       </c>
-      <c r="L64" t="s">
-        <v>90</v>
-      </c>
-      <c r="N64" t="s">
-        <v>148</v>
-      </c>
       <c r="O64" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
@@ -4457,10 +4454,10 @@
         <v>125</v>
       </c>
       <c r="B65" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" t="s">
         <v>133</v>
-      </c>
-      <c r="C65" t="s">
-        <v>134</v>
       </c>
       <c r="D65">
         <v>350.07</v>
@@ -4481,16 +4478,16 @@
         <v>16</v>
       </c>
       <c r="K65" t="s">
+        <v>146</v>
+      </c>
+      <c r="L65" t="s">
+        <v>90</v>
+      </c>
+      <c r="N65" t="s">
         <v>147</v>
       </c>
-      <c r="L65" t="s">
-        <v>90</v>
-      </c>
-      <c r="N65" t="s">
-        <v>148</v>
-      </c>
       <c r="O65" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
@@ -4498,10 +4495,10 @@
         <v>125</v>
       </c>
       <c r="B66" t="s">
+        <v>134</v>
+      </c>
+      <c r="C66" t="s">
         <v>135</v>
-      </c>
-      <c r="C66" t="s">
-        <v>136</v>
       </c>
       <c r="D66">
         <v>232.36</v>
@@ -4522,16 +4519,16 @@
         <v>16</v>
       </c>
       <c r="K66" t="s">
+        <v>146</v>
+      </c>
+      <c r="L66" t="s">
+        <v>90</v>
+      </c>
+      <c r="N66" t="s">
         <v>147</v>
       </c>
-      <c r="L66" t="s">
-        <v>90</v>
-      </c>
-      <c r="N66" t="s">
-        <v>148</v>
-      </c>
       <c r="O66" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
@@ -4539,10 +4536,10 @@
         <v>125</v>
       </c>
       <c r="B67" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C67" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D67">
         <v>238.01</v>
@@ -4563,16 +4560,16 @@
         <v>16</v>
       </c>
       <c r="K67" t="s">
+        <v>146</v>
+      </c>
+      <c r="L67" t="s">
+        <v>90</v>
+      </c>
+      <c r="N67" t="s">
         <v>147</v>
       </c>
-      <c r="L67" t="s">
-        <v>90</v>
-      </c>
-      <c r="N67" t="s">
-        <v>148</v>
-      </c>
       <c r="O67" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
@@ -4580,10 +4577,10 @@
         <v>125</v>
       </c>
       <c r="B68" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D68">
         <v>172.1</v>
@@ -4604,16 +4601,16 @@
         <v>16</v>
       </c>
       <c r="K68" t="s">
+        <v>146</v>
+      </c>
+      <c r="L68" t="s">
+        <v>90</v>
+      </c>
+      <c r="N68" t="s">
         <v>147</v>
       </c>
-      <c r="L68" t="s">
-        <v>90</v>
-      </c>
-      <c r="N68" t="s">
-        <v>148</v>
-      </c>
       <c r="O68" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
@@ -4621,10 +4618,10 @@
         <v>125</v>
       </c>
       <c r="B69" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C69" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D69">
         <v>308.5</v>
@@ -4645,16 +4642,16 @@
         <v>16</v>
       </c>
       <c r="K69" t="s">
+        <v>146</v>
+      </c>
+      <c r="L69" t="s">
+        <v>90</v>
+      </c>
+      <c r="N69" t="s">
         <v>147</v>
       </c>
-      <c r="L69" t="s">
-        <v>90</v>
-      </c>
-      <c r="N69" t="s">
-        <v>148</v>
-      </c>
       <c r="O69" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
@@ -4662,10 +4659,10 @@
         <v>125</v>
       </c>
       <c r="B70" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C70" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D70">
         <v>238.81</v>
@@ -4686,16 +4683,16 @@
         <v>16</v>
       </c>
       <c r="K70" t="s">
+        <v>146</v>
+      </c>
+      <c r="L70" t="s">
+        <v>90</v>
+      </c>
+      <c r="N70" t="s">
         <v>147</v>
       </c>
-      <c r="L70" t="s">
-        <v>90</v>
-      </c>
-      <c r="N70" t="s">
-        <v>148</v>
-      </c>
       <c r="O70" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
@@ -4703,10 +4700,10 @@
         <v>125</v>
       </c>
       <c r="B71" t="s">
+        <v>140</v>
+      </c>
+      <c r="C71" t="s">
         <v>141</v>
-      </c>
-      <c r="C71" t="s">
-        <v>142</v>
       </c>
       <c r="D71">
         <v>101.08</v>
@@ -4727,16 +4724,16 @@
         <v>16</v>
       </c>
       <c r="K71" t="s">
+        <v>146</v>
+      </c>
+      <c r="L71" t="s">
+        <v>90</v>
+      </c>
+      <c r="N71" t="s">
         <v>147</v>
       </c>
-      <c r="L71" t="s">
-        <v>90</v>
-      </c>
-      <c r="N71" t="s">
-        <v>148</v>
-      </c>
       <c r="O71" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
@@ -4744,10 +4741,10 @@
         <v>125</v>
       </c>
       <c r="B72" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C72" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D72">
         <v>170.89</v>
@@ -4768,16 +4765,16 @@
         <v>16</v>
       </c>
       <c r="K72" t="s">
+        <v>146</v>
+      </c>
+      <c r="L72" t="s">
+        <v>90</v>
+      </c>
+      <c r="N72" t="s">
         <v>147</v>
       </c>
-      <c r="L72" t="s">
-        <v>90</v>
-      </c>
-      <c r="N72" t="s">
-        <v>148</v>
-      </c>
       <c r="O72" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
@@ -4785,10 +4782,10 @@
         <v>125</v>
       </c>
       <c r="B73" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C73" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D73">
         <v>237.97</v>
@@ -4809,16 +4806,16 @@
         <v>16</v>
       </c>
       <c r="K73" t="s">
+        <v>146</v>
+      </c>
+      <c r="L73" t="s">
+        <v>90</v>
+      </c>
+      <c r="N73" t="s">
         <v>147</v>
       </c>
-      <c r="L73" t="s">
-        <v>90</v>
-      </c>
-      <c r="N73" t="s">
-        <v>148</v>
-      </c>
       <c r="O73" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
@@ -4826,10 +4823,10 @@
         <v>125</v>
       </c>
       <c r="B74" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C74" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D74">
         <v>237.57</v>
@@ -4850,16 +4847,16 @@
         <v>16</v>
       </c>
       <c r="K74" t="s">
+        <v>146</v>
+      </c>
+      <c r="L74" t="s">
+        <v>90</v>
+      </c>
+      <c r="N74" t="s">
         <v>147</v>
       </c>
-      <c r="L74" t="s">
-        <v>90</v>
-      </c>
-      <c r="N74" t="s">
-        <v>148</v>
-      </c>
       <c r="O74" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
@@ -4867,10 +4864,10 @@
         <v>125</v>
       </c>
       <c r="B75" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C75" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D75">
         <v>318.95999999999998</v>
@@ -4891,16 +4888,16 @@
         <v>16</v>
       </c>
       <c r="K75" t="s">
+        <v>146</v>
+      </c>
+      <c r="L75" t="s">
+        <v>90</v>
+      </c>
+      <c r="N75" t="s">
         <v>147</v>
       </c>
-      <c r="L75" t="s">
-        <v>90</v>
-      </c>
-      <c r="N75" t="s">
-        <v>148</v>
-      </c>
       <c r="O75" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
@@ -4944,10 +4941,10 @@
         <v>30</v>
       </c>
       <c r="N76" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O76" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
@@ -4958,7 +4955,7 @@
         <v>43</v>
       </c>
       <c r="C77" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D77">
         <v>511.6</v>
@@ -4991,10 +4988,10 @@
         <v>30</v>
       </c>
       <c r="N77" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O77" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
@@ -5005,7 +5002,7 @@
         <v>43</v>
       </c>
       <c r="C78" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D78">
         <v>442.2</v>
@@ -5038,10 +5035,10 @@
         <v>30</v>
       </c>
       <c r="N78" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O78" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
@@ -5052,7 +5049,7 @@
         <v>17</v>
       </c>
       <c r="C79" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D79">
         <v>34</v>
@@ -5076,21 +5073,21 @@
         <v>31</v>
       </c>
       <c r="N79" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O79" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B80" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D80">
         <v>38</v>
@@ -5120,24 +5117,24 @@
         <v>90</v>
       </c>
       <c r="M80" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N80" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O80" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C81" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D81">
         <v>33.299999999999997</v>
@@ -5167,24 +5164,24 @@
         <v>90</v>
       </c>
       <c r="M81" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N81" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O81" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B82" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C82" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D82">
         <v>31.62</v>
@@ -5214,13 +5211,13 @@
         <v>90</v>
       </c>
       <c r="M82" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N82" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O82" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
@@ -5264,21 +5261,21 @@
         <v>49</v>
       </c>
       <c r="N83" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O83" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B84" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C84" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D84">
         <v>118.8</v>
@@ -5296,30 +5293,30 @@
         <v>16</v>
       </c>
       <c r="K84" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L84" t="s">
         <v>90</v>
       </c>
       <c r="M84" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N84" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O84" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B85" t="s">
+        <v>164</v>
+      </c>
+      <c r="C85" t="s">
         <v>165</v>
-      </c>
-      <c r="C85" t="s">
-        <v>166</v>
       </c>
       <c r="D85">
         <v>103.8</v>
@@ -5337,30 +5334,30 @@
         <v>16</v>
       </c>
       <c r="K85" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L85" t="s">
         <v>90</v>
       </c>
       <c r="M85" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N85" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O85" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B86" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C86" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D86">
         <v>93.6</v>
@@ -5378,30 +5375,30 @@
         <v>16</v>
       </c>
       <c r="K86" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L86" t="s">
         <v>90</v>
       </c>
       <c r="M86" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N86" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O86" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B87" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C87" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D87">
         <v>111.5</v>
@@ -5419,30 +5416,30 @@
         <v>16</v>
       </c>
       <c r="K87" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L87" t="s">
         <v>90</v>
       </c>
       <c r="M87" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N87" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O87" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B88" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C88" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D88">
         <v>84.7</v>
@@ -5460,30 +5457,30 @@
         <v>16</v>
       </c>
       <c r="K88" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L88" t="s">
         <v>90</v>
       </c>
       <c r="M88" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N88" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O88" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B89" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C89" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D89">
         <v>97.2</v>
@@ -5501,30 +5498,30 @@
         <v>16</v>
       </c>
       <c r="K89" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L89" t="s">
         <v>90</v>
       </c>
       <c r="M89" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N89" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O89" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B90" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C90" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D90">
         <v>107.3</v>
@@ -5542,19 +5539,19 @@
         <v>16</v>
       </c>
       <c r="K90" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L90" t="s">
         <v>90</v>
       </c>
       <c r="M90" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N90" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O90" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
@@ -5565,7 +5562,7 @@
         <v>130</v>
       </c>
       <c r="C91" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D91">
         <v>53.2</v>
@@ -5595,10 +5592,10 @@
         <v>31</v>
       </c>
       <c r="N91" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O91" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
@@ -5609,7 +5606,7 @@
         <v>130</v>
       </c>
       <c r="C92" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D92">
         <v>34.4</v>
@@ -5639,10 +5636,10 @@
         <v>31</v>
       </c>
       <c r="N92" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O92" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
@@ -5650,10 +5647,10 @@
         <v>125</v>
       </c>
       <c r="B93" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C93" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D93">
         <v>32.700000000000003</v>
@@ -5683,10 +5680,10 @@
         <v>31</v>
       </c>
       <c r="N93" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O93" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
@@ -5694,10 +5691,10 @@
         <v>125</v>
       </c>
       <c r="B94" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C94" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D94">
         <v>53.5</v>
@@ -5727,10 +5724,10 @@
         <v>31</v>
       </c>
       <c r="N94" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O94" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
@@ -5771,13 +5768,13 @@
         <v>94</v>
       </c>
       <c r="M95" t="s">
+        <v>180</v>
+      </c>
+      <c r="N95" t="s">
         <v>181</v>
       </c>
-      <c r="N95" t="s">
-        <v>182</v>
-      </c>
       <c r="O95" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
@@ -5818,13 +5815,13 @@
         <v>93</v>
       </c>
       <c r="M96" t="s">
+        <v>180</v>
+      </c>
+      <c r="N96" t="s">
         <v>181</v>
       </c>
-      <c r="N96" t="s">
-        <v>182</v>
-      </c>
       <c r="O96" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
@@ -5853,19 +5850,19 @@
         <v>16</v>
       </c>
       <c r="K97" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L97" t="s">
         <v>90</v>
       </c>
       <c r="M97" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N97" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O97" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
@@ -5894,19 +5891,19 @@
         <v>16</v>
       </c>
       <c r="K98" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L98" t="s">
         <v>90</v>
       </c>
       <c r="M98" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N98" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O98" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
@@ -5917,7 +5914,7 @@
         <v>130</v>
       </c>
       <c r="C99" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D99">
         <v>192.61</v>
@@ -5935,19 +5932,19 @@
         <v>16</v>
       </c>
       <c r="K99" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L99" t="s">
         <v>90</v>
       </c>
       <c r="M99" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N99" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O99" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
@@ -5958,7 +5955,7 @@
         <v>130</v>
       </c>
       <c r="C100" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D100">
         <v>158.21</v>
@@ -5976,19 +5973,19 @@
         <v>16</v>
       </c>
       <c r="K100" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L100" t="s">
         <v>90</v>
       </c>
       <c r="M100" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N100" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O100" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
@@ -5996,10 +5993,10 @@
         <v>125</v>
       </c>
       <c r="B101" t="s">
+        <v>134</v>
+      </c>
+      <c r="C101" t="s">
         <v>135</v>
-      </c>
-      <c r="C101" t="s">
-        <v>136</v>
       </c>
       <c r="D101">
         <v>255.43</v>
@@ -6017,19 +6014,19 @@
         <v>16</v>
       </c>
       <c r="K101" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L101" t="s">
         <v>90</v>
       </c>
       <c r="M101" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N101" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O101" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
@@ -6037,10 +6034,10 @@
         <v>125</v>
       </c>
       <c r="B102" t="s">
+        <v>134</v>
+      </c>
+      <c r="C102" t="s">
         <v>135</v>
-      </c>
-      <c r="C102" t="s">
-        <v>136</v>
       </c>
       <c r="D102">
         <v>195.92</v>
@@ -6058,19 +6055,19 @@
         <v>16</v>
       </c>
       <c r="K102" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L102" t="s">
         <v>90</v>
       </c>
       <c r="M102" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N102" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O102" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
@@ -6078,10 +6075,10 @@
         <v>125</v>
       </c>
       <c r="B103" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C103" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D103">
         <v>238.36</v>
@@ -6099,19 +6096,19 @@
         <v>16</v>
       </c>
       <c r="K103" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L103" t="s">
         <v>90</v>
       </c>
       <c r="M103" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N103" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O103" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
@@ -6119,10 +6116,10 @@
         <v>125</v>
       </c>
       <c r="B104" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C104" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D104">
         <v>177.29</v>
@@ -6140,30 +6137,30 @@
         <v>16</v>
       </c>
       <c r="K104" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L104" t="s">
         <v>90</v>
       </c>
       <c r="M104" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N104" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O104" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>185</v>
+      </c>
+      <c r="B105" t="s">
         <v>186</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>187</v>
-      </c>
-      <c r="C105" t="s">
-        <v>188</v>
       </c>
       <c r="D105">
         <v>108.6</v>
@@ -6190,24 +6187,24 @@
         <v>90</v>
       </c>
       <c r="M105" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N105" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O105" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>185</v>
+      </c>
+      <c r="B106" t="s">
         <v>186</v>
       </c>
-      <c r="B106" t="s">
-        <v>187</v>
-      </c>
       <c r="C106" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D106">
         <v>90.7</v>
@@ -6234,24 +6231,24 @@
         <v>90</v>
       </c>
       <c r="M106" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N106" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O106" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>185</v>
+      </c>
+      <c r="B107" t="s">
         <v>186</v>
       </c>
-      <c r="B107" t="s">
-        <v>187</v>
-      </c>
       <c r="C107" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D107">
         <v>106.9</v>
@@ -6278,24 +6275,24 @@
         <v>90</v>
       </c>
       <c r="M107" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N107" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O107" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>185</v>
+      </c>
+      <c r="B108" t="s">
         <v>186</v>
       </c>
-      <c r="B108" t="s">
-        <v>187</v>
-      </c>
       <c r="C108" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D108">
         <v>111.3</v>
@@ -6322,24 +6319,24 @@
         <v>90</v>
       </c>
       <c r="M108" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N108" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O108" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>193</v>
+      </c>
+      <c r="B109" t="s">
         <v>194</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>195</v>
-      </c>
-      <c r="C109" t="s">
-        <v>196</v>
       </c>
       <c r="D109">
         <v>897</v>
@@ -6363,7 +6360,7 @@
         <v>16</v>
       </c>
       <c r="K109" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L109" t="s">
         <v>90</v>
@@ -6372,21 +6369,21 @@
         <v>31</v>
       </c>
       <c r="N109" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O109" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>193</v>
+      </c>
+      <c r="B110" t="s">
         <v>194</v>
       </c>
-      <c r="B110" t="s">
-        <v>195</v>
-      </c>
       <c r="C110" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D110">
         <v>1838</v>
@@ -6410,7 +6407,7 @@
         <v>16</v>
       </c>
       <c r="K110" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L110" t="s">
         <v>90</v>
@@ -6419,10 +6416,10 @@
         <v>31</v>
       </c>
       <c r="N110" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O110" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
@@ -6466,10 +6463,10 @@
         <v>99</v>
       </c>
       <c r="N111" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O111" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
@@ -6513,10 +6510,10 @@
         <v>99</v>
       </c>
       <c r="N112" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O112" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
@@ -6527,7 +6524,7 @@
         <v>43</v>
       </c>
       <c r="C113" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D113">
         <v>326.28399999999999</v>
@@ -6560,10 +6557,10 @@
         <v>99</v>
       </c>
       <c r="N113" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O113" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
@@ -6574,7 +6571,7 @@
         <v>43</v>
       </c>
       <c r="C114" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D114">
         <v>281.81400000000002</v>
@@ -6607,10 +6604,10 @@
         <v>99</v>
       </c>
       <c r="N114" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O114" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
@@ -6621,7 +6618,7 @@
         <v>43</v>
       </c>
       <c r="C115" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D115">
         <v>326.59500000000003</v>
@@ -6654,10 +6651,10 @@
         <v>99</v>
       </c>
       <c r="N115" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O115" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
@@ -6668,7 +6665,7 @@
         <v>43</v>
       </c>
       <c r="C116" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D116">
         <v>638.68299999999999</v>
@@ -6701,10 +6698,10 @@
         <v>99</v>
       </c>
       <c r="N116" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O116" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
@@ -6715,7 +6712,7 @@
         <v>43</v>
       </c>
       <c r="C117" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D117">
         <v>787.18600000000004</v>
@@ -6748,10 +6745,10 @@
         <v>99</v>
       </c>
       <c r="N117" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
@@ -6795,10 +6792,10 @@
         <v>99</v>
       </c>
       <c r="N118" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O118" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
@@ -6809,7 +6806,7 @@
         <v>76</v>
       </c>
       <c r="C119" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D119">
         <v>420.03300000000002</v>
@@ -6842,10 +6839,10 @@
         <v>99</v>
       </c>
       <c r="N119" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O119" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
@@ -6856,7 +6853,7 @@
         <v>76</v>
       </c>
       <c r="C120" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D120">
         <v>262.21600000000001</v>
@@ -6889,10 +6886,10 @@
         <v>99</v>
       </c>
       <c r="N120" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O120" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
@@ -6903,7 +6900,7 @@
         <v>76</v>
       </c>
       <c r="C121" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D121">
         <v>189.655</v>
@@ -6933,10 +6930,10 @@
         <v>99</v>
       </c>
       <c r="N121" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O121" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
@@ -6947,7 +6944,7 @@
         <v>76</v>
       </c>
       <c r="C122" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D122">
         <v>311.29399999999998</v>
@@ -6980,10 +6977,10 @@
         <v>99</v>
       </c>
       <c r="N122" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O122" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
@@ -7018,10 +7015,10 @@
         <v>99</v>
       </c>
       <c r="N123" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O123" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
@@ -7056,10 +7053,10 @@
         <v>99</v>
       </c>
       <c r="N124" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O124" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
@@ -7070,7 +7067,7 @@
         <v>108</v>
       </c>
       <c r="C125" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D125">
         <v>80</v>
@@ -7085,19 +7082,19 @@
         <v>16</v>
       </c>
       <c r="K125" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L125" t="s">
         <v>90</v>
       </c>
       <c r="M125" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N125" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O125" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
@@ -7108,7 +7105,7 @@
         <v>108</v>
       </c>
       <c r="C126" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D126">
         <v>78</v>
@@ -7123,19 +7120,19 @@
         <v>16</v>
       </c>
       <c r="K126" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L126" t="s">
         <v>90</v>
       </c>
       <c r="M126" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N126" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O126" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.25">
@@ -7146,7 +7143,7 @@
         <v>108</v>
       </c>
       <c r="C127" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D127">
         <v>89</v>
@@ -7161,19 +7158,19 @@
         <v>16</v>
       </c>
       <c r="K127" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L127" t="s">
         <v>90</v>
       </c>
       <c r="M127" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N127" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O127" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.25">
@@ -7184,7 +7181,7 @@
         <v>108</v>
       </c>
       <c r="C128" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D128">
         <v>78</v>
@@ -7199,19 +7196,19 @@
         <v>16</v>
       </c>
       <c r="K128" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L128" t="s">
         <v>90</v>
       </c>
       <c r="M128" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N128" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O128" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.25">
@@ -7222,7 +7219,7 @@
         <v>108</v>
       </c>
       <c r="C129" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D129">
         <v>84</v>
@@ -7237,19 +7234,19 @@
         <v>16</v>
       </c>
       <c r="K129" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L129" t="s">
         <v>90</v>
       </c>
       <c r="M129" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N129" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O129" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.25">
@@ -7260,7 +7257,7 @@
         <v>108</v>
       </c>
       <c r="C130" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D130">
         <v>78</v>
@@ -7275,19 +7272,19 @@
         <v>16</v>
       </c>
       <c r="K130" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L130" t="s">
         <v>90</v>
       </c>
       <c r="M130" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N130" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O130" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.25">
@@ -7313,19 +7310,19 @@
         <v>16</v>
       </c>
       <c r="K131" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L131" t="s">
         <v>90</v>
       </c>
       <c r="M131" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N131" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O131" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.25">
@@ -7351,19 +7348,19 @@
         <v>16</v>
       </c>
       <c r="K132" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L132" t="s">
         <v>90</v>
       </c>
       <c r="M132" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N132" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O132" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.25">
@@ -7389,19 +7386,19 @@
         <v>16</v>
       </c>
       <c r="K133" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L133" t="s">
         <v>90</v>
       </c>
       <c r="M133" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N133" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O133" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.25">
@@ -7427,19 +7424,19 @@
         <v>16</v>
       </c>
       <c r="K134" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L134" t="s">
         <v>90</v>
       </c>
       <c r="M134" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N134" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O134" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.25">
@@ -7465,19 +7462,19 @@
         <v>16</v>
       </c>
       <c r="K135" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L135" t="s">
         <v>90</v>
       </c>
       <c r="M135" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N135" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O135" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.25">
@@ -7503,30 +7500,30 @@
         <v>16</v>
       </c>
       <c r="K136" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L136" t="s">
         <v>90</v>
       </c>
       <c r="M136" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N136" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O136" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B137" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C137" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D137">
         <v>157</v>
@@ -7541,30 +7538,30 @@
         <v>16</v>
       </c>
       <c r="K137" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L137" t="s">
         <v>90</v>
       </c>
       <c r="M137" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N137" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O137" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B138" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C138" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D138">
         <v>135</v>
@@ -7579,30 +7576,30 @@
         <v>16</v>
       </c>
       <c r="K138" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L138" t="s">
         <v>90</v>
       </c>
       <c r="M138" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N138" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O138" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B139" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C139" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D139">
         <v>173</v>
@@ -7617,30 +7614,30 @@
         <v>16</v>
       </c>
       <c r="K139" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L139" t="s">
         <v>90</v>
       </c>
       <c r="M139" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N139" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O139" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B140" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C140" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D140">
         <v>135</v>
@@ -7655,30 +7652,30 @@
         <v>16</v>
       </c>
       <c r="K140" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L140" t="s">
         <v>90</v>
       </c>
       <c r="M140" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N140" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O140" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B141" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C141" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D141">
         <v>135</v>
@@ -7693,19 +7690,19 @@
         <v>16</v>
       </c>
       <c r="K141" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L141" t="s">
         <v>90</v>
       </c>
       <c r="M141" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N141" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O141" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.25">
@@ -7734,19 +7731,19 @@
         <v>16</v>
       </c>
       <c r="K142" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L142" t="s">
         <v>90</v>
       </c>
       <c r="M142" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N142" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O142" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.25">
@@ -7787,24 +7784,24 @@
         <v>90</v>
       </c>
       <c r="M143" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N143" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O143" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>223</v>
+      </c>
+      <c r="B144" t="s">
         <v>224</v>
       </c>
-      <c r="B144" t="s">
+      <c r="C144" t="s">
         <v>225</v>
-      </c>
-      <c r="C144" t="s">
-        <v>226</v>
       </c>
       <c r="D144">
         <v>198.94</v>
@@ -7828,19 +7825,19 @@
         <v>16</v>
       </c>
       <c r="K144" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L144" t="s">
         <v>90</v>
       </c>
       <c r="M144" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N144" t="s">
+        <v>219</v>
+      </c>
+      <c r="O144" t="s">
         <v>220</v>
-      </c>
-      <c r="O144" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.25">
@@ -7872,19 +7869,19 @@
         <v>36</v>
       </c>
       <c r="K145" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L145" t="s">
         <v>90</v>
       </c>
       <c r="M145" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N145" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O145" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="146" spans="1:15" x14ac:dyDescent="0.25">
@@ -7925,13 +7922,13 @@
         <v>90</v>
       </c>
       <c r="M146" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N146" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O146" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.25">
@@ -7942,7 +7939,7 @@
         <v>130</v>
       </c>
       <c r="C147" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D147">
         <v>46.8</v>
@@ -7963,19 +7960,19 @@
         <v>36</v>
       </c>
       <c r="K147" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L147" t="s">
         <v>90</v>
       </c>
       <c r="M147" t="s">
+        <v>229</v>
+      </c>
+      <c r="N147" t="s">
         <v>230</v>
       </c>
-      <c r="N147" t="s">
-        <v>231</v>
-      </c>
       <c r="O147" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.25">
@@ -7983,10 +7980,10 @@
         <v>125</v>
       </c>
       <c r="B148" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C148" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D148">
         <v>42.9</v>
@@ -8007,19 +8004,19 @@
         <v>36</v>
       </c>
       <c r="K148" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L148" t="s">
         <v>90</v>
       </c>
       <c r="M148" t="s">
+        <v>229</v>
+      </c>
+      <c r="N148" t="s">
         <v>230</v>
       </c>
-      <c r="N148" t="s">
-        <v>231</v>
-      </c>
       <c r="O148" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.25">
@@ -8030,7 +8027,7 @@
         <v>130</v>
       </c>
       <c r="C149" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D149">
         <v>25.6</v>
@@ -8048,19 +8045,19 @@
         <v>36</v>
       </c>
       <c r="K149" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L149" t="s">
         <v>90</v>
       </c>
       <c r="M149" t="s">
+        <v>229</v>
+      </c>
+      <c r="N149" t="s">
         <v>230</v>
       </c>
-      <c r="N149" t="s">
-        <v>231</v>
-      </c>
       <c r="O149" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.25">
@@ -8068,10 +8065,10 @@
         <v>125</v>
       </c>
       <c r="B150" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C150" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D150">
         <v>21.7</v>
@@ -8089,19 +8086,19 @@
         <v>36</v>
       </c>
       <c r="K150" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L150" t="s">
         <v>90</v>
       </c>
       <c r="M150" t="s">
+        <v>229</v>
+      </c>
+      <c r="N150" t="s">
         <v>230</v>
       </c>
-      <c r="N150" t="s">
-        <v>231</v>
-      </c>
       <c r="O150" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.25">
@@ -8112,7 +8109,7 @@
         <v>43</v>
       </c>
       <c r="C151" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D151">
         <v>282.13</v>
@@ -8142,10 +8139,10 @@
         <v>99</v>
       </c>
       <c r="N151" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O151" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="152" spans="1:15" x14ac:dyDescent="0.25">
@@ -8156,7 +8153,7 @@
         <v>43</v>
       </c>
       <c r="C152" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D152">
         <v>274.60000000000002</v>
@@ -8183,13 +8180,13 @@
         <v>90</v>
       </c>
       <c r="M152" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N152" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O152" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="153" spans="1:15" x14ac:dyDescent="0.25">
@@ -8230,10 +8227,10 @@
         <v>99</v>
       </c>
       <c r="N153" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O153" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="154" spans="1:15" x14ac:dyDescent="0.25">
@@ -8271,13 +8268,13 @@
         <v>90</v>
       </c>
       <c r="M154" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N154" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O154" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="155" spans="1:15" x14ac:dyDescent="0.25">
@@ -8318,10 +8315,10 @@
         <v>99</v>
       </c>
       <c r="N155" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O155" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="156" spans="1:15" x14ac:dyDescent="0.25">
@@ -8359,13 +8356,13 @@
         <v>90</v>
       </c>
       <c r="M156" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N156" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O156" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="157" spans="1:15" x14ac:dyDescent="0.25">
@@ -8376,7 +8373,7 @@
         <v>17</v>
       </c>
       <c r="C157" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D157">
         <v>296</v>
@@ -8403,24 +8400,24 @@
         <v>90</v>
       </c>
       <c r="M157" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N157" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O157" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B158" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C158" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D158">
         <v>308</v>
@@ -8447,13 +8444,13 @@
         <v>90</v>
       </c>
       <c r="M158" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N158" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O158" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="159" spans="1:15" x14ac:dyDescent="0.25">
@@ -8491,13 +8488,13 @@
         <v>90</v>
       </c>
       <c r="M159" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N159" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O159" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="160" spans="1:15" x14ac:dyDescent="0.25">
@@ -8535,13 +8532,13 @@
         <v>90</v>
       </c>
       <c r="M160" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N160" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O160" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.25">
@@ -8549,10 +8546,10 @@
         <v>125</v>
       </c>
       <c r="B161" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C161" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D161">
         <v>263</v>
@@ -8582,13 +8579,13 @@
         <v>90</v>
       </c>
       <c r="M161" t="s">
+        <v>239</v>
+      </c>
+      <c r="N161" t="s">
         <v>240</v>
       </c>
-      <c r="N161" t="s">
-        <v>241</v>
-      </c>
       <c r="O161" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.25">
@@ -8599,7 +8596,7 @@
         <v>128</v>
       </c>
       <c r="C162" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D162">
         <v>402</v>
@@ -8629,13 +8626,13 @@
         <v>90</v>
       </c>
       <c r="M162" t="s">
+        <v>239</v>
+      </c>
+      <c r="N162" t="s">
         <v>240</v>
       </c>
-      <c r="N162" t="s">
-        <v>241</v>
-      </c>
       <c r="O162" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.25">
@@ -8646,7 +8643,7 @@
         <v>130</v>
       </c>
       <c r="C163" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D163">
         <v>372</v>
@@ -8676,13 +8673,13 @@
         <v>90</v>
       </c>
       <c r="M163" t="s">
+        <v>239</v>
+      </c>
+      <c r="N163" t="s">
         <v>240</v>
       </c>
-      <c r="N163" t="s">
-        <v>241</v>
-      </c>
       <c r="O163" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="164" spans="1:15" x14ac:dyDescent="0.25">
@@ -8693,7 +8690,7 @@
         <v>130</v>
       </c>
       <c r="C164" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D164">
         <v>457</v>
@@ -8723,13 +8720,13 @@
         <v>90</v>
       </c>
       <c r="M164" t="s">
+        <v>239</v>
+      </c>
+      <c r="N164" t="s">
         <v>240</v>
       </c>
-      <c r="N164" t="s">
-        <v>241</v>
-      </c>
       <c r="O164" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="165" spans="1:15" x14ac:dyDescent="0.25">
@@ -8740,7 +8737,7 @@
         <v>130</v>
       </c>
       <c r="C165" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D165">
         <v>218</v>
@@ -8770,13 +8767,13 @@
         <v>90</v>
       </c>
       <c r="M165" t="s">
+        <v>239</v>
+      </c>
+      <c r="N165" t="s">
         <v>240</v>
       </c>
-      <c r="N165" t="s">
-        <v>241</v>
-      </c>
       <c r="O165" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="166" spans="1:15" x14ac:dyDescent="0.25">
@@ -8784,10 +8781,10 @@
         <v>125</v>
       </c>
       <c r="B166" t="s">
+        <v>132</v>
+      </c>
+      <c r="C166" t="s">
         <v>133</v>
-      </c>
-      <c r="C166" t="s">
-        <v>134</v>
       </c>
       <c r="D166">
         <v>366</v>
@@ -8817,13 +8814,13 @@
         <v>90</v>
       </c>
       <c r="M166" t="s">
+        <v>239</v>
+      </c>
+      <c r="N166" t="s">
         <v>240</v>
       </c>
-      <c r="N166" t="s">
-        <v>241</v>
-      </c>
       <c r="O166" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.25">
@@ -8831,10 +8828,10 @@
         <v>125</v>
       </c>
       <c r="B167" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C167" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D167">
         <v>339</v>
@@ -8864,13 +8861,13 @@
         <v>90</v>
       </c>
       <c r="M167" t="s">
+        <v>239</v>
+      </c>
+      <c r="N167" t="s">
         <v>240</v>
       </c>
-      <c r="N167" t="s">
-        <v>241</v>
-      </c>
       <c r="O167" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.25">
@@ -8878,10 +8875,10 @@
         <v>125</v>
       </c>
       <c r="B168" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C168" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D168">
         <v>281</v>
@@ -8911,13 +8908,13 @@
         <v>90</v>
       </c>
       <c r="M168" t="s">
+        <v>239</v>
+      </c>
+      <c r="N168" t="s">
         <v>240</v>
       </c>
-      <c r="N168" t="s">
-        <v>241</v>
-      </c>
       <c r="O168" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="169" spans="1:15" x14ac:dyDescent="0.25">
@@ -8925,10 +8922,10 @@
         <v>125</v>
       </c>
       <c r="B169" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C169" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D169">
         <v>310</v>
@@ -8958,13 +8955,13 @@
         <v>90</v>
       </c>
       <c r="M169" t="s">
+        <v>239</v>
+      </c>
+      <c r="N169" t="s">
         <v>240</v>
       </c>
-      <c r="N169" t="s">
-        <v>241</v>
-      </c>
       <c r="O169" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="170" spans="1:15" x14ac:dyDescent="0.25">
@@ -8972,10 +8969,10 @@
         <v>125</v>
       </c>
       <c r="B170" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C170" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D170">
         <v>207</v>
@@ -9005,13 +9002,13 @@
         <v>90</v>
       </c>
       <c r="M170" t="s">
+        <v>239</v>
+      </c>
+      <c r="N170" t="s">
         <v>240</v>
       </c>
-      <c r="N170" t="s">
-        <v>241</v>
-      </c>
       <c r="O170" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.25">
@@ -9019,10 +9016,10 @@
         <v>125</v>
       </c>
       <c r="B171" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C171" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D171">
         <v>376</v>
@@ -9052,13 +9049,13 @@
         <v>90</v>
       </c>
       <c r="M171" t="s">
+        <v>239</v>
+      </c>
+      <c r="N171" t="s">
         <v>240</v>
       </c>
-      <c r="N171" t="s">
-        <v>241</v>
-      </c>
       <c r="O171" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="172" spans="1:15" x14ac:dyDescent="0.25">
@@ -9066,10 +9063,10 @@
         <v>125</v>
       </c>
       <c r="B172" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C172" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D172">
         <v>252</v>
@@ -9099,24 +9096,24 @@
         <v>90</v>
       </c>
       <c r="M172" t="s">
+        <v>239</v>
+      </c>
+      <c r="N172" t="s">
         <v>240</v>
       </c>
-      <c r="N172" t="s">
-        <v>241</v>
-      </c>
       <c r="O172" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="173" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>185</v>
+      </c>
+      <c r="B173" t="s">
         <v>186</v>
       </c>
-      <c r="B173" t="s">
-        <v>187</v>
-      </c>
       <c r="C173" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D173">
         <v>11</v>
@@ -9146,13 +9143,13 @@
         <v>90</v>
       </c>
       <c r="M173" t="s">
+        <v>249</v>
+      </c>
+      <c r="N173" t="s">
         <v>250</v>
       </c>
-      <c r="N173" t="s">
-        <v>251</v>
-      </c>
       <c r="O173" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="174" spans="1:15" x14ac:dyDescent="0.25">
@@ -9163,7 +9160,7 @@
         <v>130</v>
       </c>
       <c r="C174" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D174">
         <v>47.38</v>
@@ -9193,13 +9190,13 @@
         <v>90</v>
       </c>
       <c r="M174" t="s">
+        <v>249</v>
+      </c>
+      <c r="N174" t="s">
         <v>250</v>
       </c>
-      <c r="N174" t="s">
-        <v>251</v>
-      </c>
       <c r="O174" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="175" spans="1:15" x14ac:dyDescent="0.25">
@@ -9240,13 +9237,13 @@
         <v>90</v>
       </c>
       <c r="M175" t="s">
+        <v>249</v>
+      </c>
+      <c r="N175" t="s">
         <v>250</v>
       </c>
-      <c r="N175" t="s">
-        <v>251</v>
-      </c>
       <c r="O175" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="176" spans="1:15" x14ac:dyDescent="0.25">
@@ -9287,13 +9284,13 @@
         <v>90</v>
       </c>
       <c r="M176" t="s">
+        <v>249</v>
+      </c>
+      <c r="N176" t="s">
         <v>250</v>
       </c>
-      <c r="N176" t="s">
-        <v>251</v>
-      </c>
       <c r="O176" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.25">
@@ -9334,13 +9331,13 @@
         <v>93</v>
       </c>
       <c r="M177" t="s">
+        <v>249</v>
+      </c>
+      <c r="N177" t="s">
         <v>250</v>
       </c>
-      <c r="N177" t="s">
-        <v>251</v>
-      </c>
       <c r="O177" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.25">
@@ -9381,13 +9378,13 @@
         <v>94</v>
       </c>
       <c r="M178" t="s">
+        <v>249</v>
+      </c>
+      <c r="N178" t="s">
         <v>250</v>
       </c>
-      <c r="N178" t="s">
-        <v>251</v>
-      </c>
       <c r="O178" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.25">
@@ -9398,7 +9395,7 @@
         <v>17</v>
       </c>
       <c r="C179" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D179">
         <v>22.37</v>
@@ -9428,13 +9425,13 @@
         <v>93</v>
       </c>
       <c r="M179" t="s">
+        <v>249</v>
+      </c>
+      <c r="N179" t="s">
         <v>250</v>
       </c>
-      <c r="N179" t="s">
-        <v>251</v>
-      </c>
       <c r="O179" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.25">
@@ -9445,7 +9442,7 @@
         <v>17</v>
       </c>
       <c r="C180" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D180">
         <v>19.75</v>
@@ -9475,13 +9472,13 @@
         <v>94</v>
       </c>
       <c r="M180" t="s">
+        <v>249</v>
+      </c>
+      <c r="N180" t="s">
         <v>250</v>
       </c>
-      <c r="N180" t="s">
-        <v>251</v>
-      </c>
       <c r="O180" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.25">
@@ -9522,13 +9519,13 @@
         <v>93</v>
       </c>
       <c r="M181" t="s">
+        <v>249</v>
+      </c>
+      <c r="N181" t="s">
         <v>250</v>
       </c>
-      <c r="N181" t="s">
-        <v>251</v>
-      </c>
       <c r="O181" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.25">
@@ -9569,24 +9566,24 @@
         <v>94</v>
       </c>
       <c r="M182" t="s">
+        <v>249</v>
+      </c>
+      <c r="N182" t="s">
         <v>250</v>
       </c>
-      <c r="N182" t="s">
-        <v>251</v>
-      </c>
       <c r="O182" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="183" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
+        <v>185</v>
+      </c>
+      <c r="B183" t="s">
         <v>186</v>
       </c>
-      <c r="B183" t="s">
-        <v>187</v>
-      </c>
       <c r="C183" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D183">
         <v>10.99</v>
@@ -9616,13 +9613,13 @@
         <v>90</v>
       </c>
       <c r="M183" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N183" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O183" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="184" spans="1:15" x14ac:dyDescent="0.25">
@@ -9663,13 +9660,13 @@
         <v>90</v>
       </c>
       <c r="M184" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N184" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O184" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="185" spans="1:15" x14ac:dyDescent="0.25">
@@ -9710,13 +9707,13 @@
         <v>93</v>
       </c>
       <c r="M185" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N185" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O185" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="186" spans="1:15" x14ac:dyDescent="0.25">
@@ -9757,13 +9754,13 @@
         <v>94</v>
       </c>
       <c r="M186" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N186" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O186" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.25">
@@ -9804,13 +9801,13 @@
         <v>93</v>
       </c>
       <c r="M187" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N187" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O187" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="188" spans="1:15" x14ac:dyDescent="0.25">
@@ -9851,24 +9848,24 @@
         <v>94</v>
       </c>
       <c r="M188" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N188" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O188" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="189" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
+        <v>185</v>
+      </c>
+      <c r="B189" t="s">
         <v>186</v>
       </c>
-      <c r="B189" t="s">
-        <v>187</v>
-      </c>
       <c r="C189" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D189">
         <v>10.7</v>
@@ -9898,13 +9895,13 @@
         <v>90</v>
       </c>
       <c r="M189" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N189" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O189" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.25">
@@ -9945,13 +9942,13 @@
         <v>90</v>
       </c>
       <c r="M190" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N190" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O190" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="191" spans="1:15" x14ac:dyDescent="0.25">
@@ -9992,13 +9989,13 @@
         <v>93</v>
       </c>
       <c r="M191" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N191" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O191" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="192" spans="1:15" x14ac:dyDescent="0.25">
@@ -10039,13 +10036,13 @@
         <v>94</v>
       </c>
       <c r="M192" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N192" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O192" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="193" spans="1:15" x14ac:dyDescent="0.25">
@@ -10086,13 +10083,13 @@
         <v>93</v>
       </c>
       <c r="M193" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N193" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O193" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.25">
@@ -10133,13 +10130,13 @@
         <v>94</v>
       </c>
       <c r="M194" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N194" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O194" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="195" spans="1:15" x14ac:dyDescent="0.25">
@@ -10180,24 +10177,24 @@
         <v>90</v>
       </c>
       <c r="M195" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N195" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O195" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="196" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
+        <v>185</v>
+      </c>
+      <c r="B196" t="s">
         <v>186</v>
       </c>
-      <c r="B196" t="s">
-        <v>187</v>
-      </c>
       <c r="C196" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D196">
         <v>10.52</v>
@@ -10227,13 +10224,13 @@
         <v>90</v>
       </c>
       <c r="M196" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N196" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O196" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="197" spans="1:15" x14ac:dyDescent="0.25">
@@ -10274,13 +10271,13 @@
         <v>90</v>
       </c>
       <c r="M197" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N197" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O197" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="198" spans="1:15" x14ac:dyDescent="0.25">
@@ -10321,13 +10318,13 @@
         <v>93</v>
       </c>
       <c r="M198" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N198" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O198" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="199" spans="1:15" x14ac:dyDescent="0.25">
@@ -10368,13 +10365,13 @@
         <v>94</v>
       </c>
       <c r="M199" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N199" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O199" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="200" spans="1:15" x14ac:dyDescent="0.25">
@@ -10415,13 +10412,13 @@
         <v>93</v>
       </c>
       <c r="M200" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O200" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="201" spans="1:15" x14ac:dyDescent="0.25">
@@ -10462,13 +10459,13 @@
         <v>94</v>
       </c>
       <c r="M201" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N201" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O201" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="202" spans="1:15" x14ac:dyDescent="0.25">
@@ -10509,13 +10506,13 @@
         <v>93</v>
       </c>
       <c r="M202" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N202" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O202" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="203" spans="1:15" x14ac:dyDescent="0.25">
@@ -10556,13 +10553,13 @@
         <v>94</v>
       </c>
       <c r="M203" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N203" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O203" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -10706,10 +10703,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replace Scaridae by Labridae for two species
</commit_message>
<xml_diff>
--- a/data/00_von-bertalanffy-literature.xlsx
+++ b/data/00_von-bertalanffy-literature.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="256">
   <si>
     <t>Family</t>
   </si>
@@ -395,9 +395,6 @@
   </si>
   <si>
     <t>Zebrasoma scopas</t>
-  </si>
-  <si>
-    <t>Scaridae</t>
   </si>
   <si>
     <t>Bolbometopon</t>
@@ -1659,7 +1656,7 @@
         <v>7</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1706,7 +1703,7 @@
         <v>12</v>
       </c>
       <c r="O2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1753,7 +1750,7 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1800,7 +1797,7 @@
         <v>37</v>
       </c>
       <c r="O4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1847,7 +1844,7 @@
         <v>40</v>
       </c>
       <c r="O5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1894,7 +1891,7 @@
         <v>48</v>
       </c>
       <c r="O6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1941,7 +1938,7 @@
         <v>48</v>
       </c>
       <c r="O7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1988,7 +1985,7 @@
         <v>48</v>
       </c>
       <c r="O8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2035,7 +2032,7 @@
         <v>48</v>
       </c>
       <c r="O9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2082,7 +2079,7 @@
         <v>48</v>
       </c>
       <c r="O10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2129,7 +2126,7 @@
         <v>48</v>
       </c>
       <c r="O11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -2176,7 +2173,7 @@
         <v>48</v>
       </c>
       <c r="O12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2223,7 +2220,7 @@
         <v>48</v>
       </c>
       <c r="O13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2270,7 +2267,7 @@
         <v>48</v>
       </c>
       <c r="O14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2317,7 +2314,7 @@
         <v>48</v>
       </c>
       <c r="O15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2364,7 +2361,7 @@
         <v>48</v>
       </c>
       <c r="O16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -2411,7 +2408,7 @@
         <v>48</v>
       </c>
       <c r="O17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -2458,7 +2455,7 @@
         <v>48</v>
       </c>
       <c r="O18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -2505,7 +2502,7 @@
         <v>48</v>
       </c>
       <c r="O19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -2552,7 +2549,7 @@
         <v>48</v>
       </c>
       <c r="O20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -2599,7 +2596,7 @@
         <v>64</v>
       </c>
       <c r="O21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2646,7 +2643,7 @@
         <v>64</v>
       </c>
       <c r="O22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -2693,7 +2690,7 @@
         <v>64</v>
       </c>
       <c r="O23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2740,7 +2737,7 @@
         <v>64</v>
       </c>
       <c r="O24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -2784,7 +2781,7 @@
         <v>68</v>
       </c>
       <c r="O25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2831,7 +2828,7 @@
         <v>74</v>
       </c>
       <c r="O26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2872,7 +2869,7 @@
         <v>75</v>
       </c>
       <c r="O27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2913,7 +2910,7 @@
         <v>75</v>
       </c>
       <c r="O28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -2957,7 +2954,7 @@
         <v>81</v>
       </c>
       <c r="O29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -3001,7 +2998,7 @@
         <v>81</v>
       </c>
       <c r="O30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -3045,7 +3042,7 @@
         <v>81</v>
       </c>
       <c r="O31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -3089,7 +3086,7 @@
         <v>81</v>
       </c>
       <c r="O32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -3133,7 +3130,7 @@
         <v>81</v>
       </c>
       <c r="O33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -3177,7 +3174,7 @@
         <v>81</v>
       </c>
       <c r="O34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -3224,7 +3221,7 @@
         <v>92</v>
       </c>
       <c r="O35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -3271,7 +3268,7 @@
         <v>92</v>
       </c>
       <c r="O36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -3318,7 +3315,7 @@
         <v>97</v>
       </c>
       <c r="O37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -3365,7 +3362,7 @@
         <v>100</v>
       </c>
       <c r="O38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -3409,7 +3406,7 @@
         <v>101</v>
       </c>
       <c r="O39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -3453,7 +3450,7 @@
         <v>101</v>
       </c>
       <c r="O40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -3497,7 +3494,7 @@
         <v>101</v>
       </c>
       <c r="O41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -3541,7 +3538,7 @@
         <v>101</v>
       </c>
       <c r="O42" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -3585,7 +3582,7 @@
         <v>101</v>
       </c>
       <c r="O43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -3617,16 +3614,16 @@
         <v>16</v>
       </c>
       <c r="K44" t="s">
+        <v>145</v>
+      </c>
+      <c r="L44" t="s">
+        <v>90</v>
+      </c>
+      <c r="N44" t="s">
         <v>146</v>
       </c>
-      <c r="L44" t="s">
-        <v>90</v>
-      </c>
-      <c r="N44" t="s">
-        <v>147</v>
-      </c>
       <c r="O44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -3658,16 +3655,16 @@
         <v>16</v>
       </c>
       <c r="K45" t="s">
+        <v>145</v>
+      </c>
+      <c r="L45" t="s">
+        <v>90</v>
+      </c>
+      <c r="N45" t="s">
         <v>146</v>
       </c>
-      <c r="L45" t="s">
-        <v>90</v>
-      </c>
-      <c r="N45" t="s">
-        <v>147</v>
-      </c>
       <c r="O45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
@@ -3699,16 +3696,16 @@
         <v>16</v>
       </c>
       <c r="K46" t="s">
+        <v>145</v>
+      </c>
+      <c r="L46" t="s">
+        <v>90</v>
+      </c>
+      <c r="N46" t="s">
         <v>146</v>
       </c>
-      <c r="L46" t="s">
-        <v>90</v>
-      </c>
-      <c r="N46" t="s">
-        <v>147</v>
-      </c>
       <c r="O46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
@@ -3740,16 +3737,16 @@
         <v>16</v>
       </c>
       <c r="K47" t="s">
+        <v>145</v>
+      </c>
+      <c r="L47" t="s">
+        <v>90</v>
+      </c>
+      <c r="N47" t="s">
         <v>146</v>
       </c>
-      <c r="L47" t="s">
-        <v>90</v>
-      </c>
-      <c r="N47" t="s">
-        <v>147</v>
-      </c>
       <c r="O47" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
@@ -3781,16 +3778,16 @@
         <v>16</v>
       </c>
       <c r="K48" t="s">
+        <v>145</v>
+      </c>
+      <c r="L48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N48" t="s">
         <v>146</v>
       </c>
-      <c r="L48" t="s">
-        <v>90</v>
-      </c>
-      <c r="N48" t="s">
-        <v>147</v>
-      </c>
       <c r="O48" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -3822,16 +3819,16 @@
         <v>16</v>
       </c>
       <c r="K49" t="s">
+        <v>145</v>
+      </c>
+      <c r="L49" t="s">
+        <v>90</v>
+      </c>
+      <c r="N49" t="s">
         <v>146</v>
       </c>
-      <c r="L49" t="s">
-        <v>90</v>
-      </c>
-      <c r="N49" t="s">
-        <v>147</v>
-      </c>
       <c r="O49" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -3863,16 +3860,16 @@
         <v>16</v>
       </c>
       <c r="K50" t="s">
+        <v>145</v>
+      </c>
+      <c r="L50" t="s">
+        <v>90</v>
+      </c>
+      <c r="N50" t="s">
         <v>146</v>
       </c>
-      <c r="L50" t="s">
-        <v>90</v>
-      </c>
-      <c r="N50" t="s">
-        <v>147</v>
-      </c>
       <c r="O50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -3904,16 +3901,16 @@
         <v>16</v>
       </c>
       <c r="K51" t="s">
+        <v>145</v>
+      </c>
+      <c r="L51" t="s">
+        <v>90</v>
+      </c>
+      <c r="N51" t="s">
         <v>146</v>
       </c>
-      <c r="L51" t="s">
-        <v>90</v>
-      </c>
-      <c r="N51" t="s">
-        <v>147</v>
-      </c>
       <c r="O51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -3945,16 +3942,16 @@
         <v>16</v>
       </c>
       <c r="K52" t="s">
+        <v>145</v>
+      </c>
+      <c r="L52" t="s">
+        <v>90</v>
+      </c>
+      <c r="N52" t="s">
         <v>146</v>
       </c>
-      <c r="L52" t="s">
-        <v>90</v>
-      </c>
-      <c r="N52" t="s">
-        <v>147</v>
-      </c>
       <c r="O52" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -3986,16 +3983,16 @@
         <v>16</v>
       </c>
       <c r="K53" t="s">
+        <v>145</v>
+      </c>
+      <c r="L53" t="s">
+        <v>90</v>
+      </c>
+      <c r="N53" t="s">
         <v>146</v>
       </c>
-      <c r="L53" t="s">
-        <v>90</v>
-      </c>
-      <c r="N53" t="s">
-        <v>147</v>
-      </c>
       <c r="O53" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -4027,16 +4024,16 @@
         <v>16</v>
       </c>
       <c r="K54" t="s">
+        <v>145</v>
+      </c>
+      <c r="L54" t="s">
+        <v>90</v>
+      </c>
+      <c r="N54" t="s">
         <v>146</v>
       </c>
-      <c r="L54" t="s">
-        <v>90</v>
-      </c>
-      <c r="N54" t="s">
-        <v>147</v>
-      </c>
       <c r="O54" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -4068,16 +4065,16 @@
         <v>16</v>
       </c>
       <c r="K55" t="s">
+        <v>145</v>
+      </c>
+      <c r="L55" t="s">
+        <v>90</v>
+      </c>
+      <c r="N55" t="s">
         <v>146</v>
       </c>
-      <c r="L55" t="s">
-        <v>90</v>
-      </c>
-      <c r="N55" t="s">
-        <v>147</v>
-      </c>
       <c r="O55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
@@ -4109,16 +4106,16 @@
         <v>16</v>
       </c>
       <c r="K56" t="s">
+        <v>145</v>
+      </c>
+      <c r="L56" t="s">
+        <v>90</v>
+      </c>
+      <c r="N56" t="s">
         <v>146</v>
       </c>
-      <c r="L56" t="s">
-        <v>90</v>
-      </c>
-      <c r="N56" t="s">
-        <v>147</v>
-      </c>
       <c r="O56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -4150,16 +4147,16 @@
         <v>16</v>
       </c>
       <c r="K57" t="s">
+        <v>145</v>
+      </c>
+      <c r="L57" t="s">
+        <v>90</v>
+      </c>
+      <c r="N57" t="s">
         <v>146</v>
       </c>
-      <c r="L57" t="s">
-        <v>90</v>
-      </c>
-      <c r="N57" t="s">
-        <v>147</v>
-      </c>
       <c r="O57" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
@@ -4191,16 +4188,16 @@
         <v>16</v>
       </c>
       <c r="K58" t="s">
+        <v>145</v>
+      </c>
+      <c r="L58" t="s">
+        <v>90</v>
+      </c>
+      <c r="N58" t="s">
         <v>146</v>
       </c>
-      <c r="L58" t="s">
-        <v>90</v>
-      </c>
-      <c r="N58" t="s">
-        <v>147</v>
-      </c>
       <c r="O58" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
@@ -4232,16 +4229,16 @@
         <v>16</v>
       </c>
       <c r="K59" t="s">
+        <v>145</v>
+      </c>
+      <c r="L59" t="s">
+        <v>90</v>
+      </c>
+      <c r="N59" t="s">
         <v>146</v>
       </c>
-      <c r="L59" t="s">
-        <v>90</v>
-      </c>
-      <c r="N59" t="s">
-        <v>147</v>
-      </c>
       <c r="O59" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
@@ -4273,27 +4270,27 @@
         <v>16</v>
       </c>
       <c r="K60" t="s">
+        <v>145</v>
+      </c>
+      <c r="L60" t="s">
+        <v>90</v>
+      </c>
+      <c r="N60" t="s">
         <v>146</v>
       </c>
-      <c r="L60" t="s">
-        <v>90</v>
-      </c>
-      <c r="N60" t="s">
-        <v>147</v>
-      </c>
       <c r="O60" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>222</v>
+      </c>
+      <c r="B61" t="s">
         <v>125</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>126</v>
-      </c>
-      <c r="C61" t="s">
-        <v>127</v>
       </c>
       <c r="D61">
         <v>693.81</v>
@@ -4314,27 +4311,27 @@
         <v>16</v>
       </c>
       <c r="K61" t="s">
+        <v>145</v>
+      </c>
+      <c r="L61" t="s">
+        <v>90</v>
+      </c>
+      <c r="N61" t="s">
         <v>146</v>
       </c>
-      <c r="L61" t="s">
-        <v>90</v>
-      </c>
-      <c r="N61" t="s">
-        <v>147</v>
-      </c>
       <c r="O61" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B62" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" t="s">
         <v>128</v>
-      </c>
-      <c r="C62" t="s">
-        <v>129</v>
       </c>
       <c r="D62">
         <v>420.56</v>
@@ -4355,27 +4352,27 @@
         <v>16</v>
       </c>
       <c r="K62" t="s">
+        <v>145</v>
+      </c>
+      <c r="L62" t="s">
+        <v>90</v>
+      </c>
+      <c r="N62" t="s">
         <v>146</v>
       </c>
-      <c r="L62" t="s">
-        <v>90</v>
-      </c>
-      <c r="N62" t="s">
-        <v>147</v>
-      </c>
       <c r="O62" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D63">
         <v>429.89</v>
@@ -4396,27 +4393,27 @@
         <v>16</v>
       </c>
       <c r="K63" t="s">
+        <v>145</v>
+      </c>
+      <c r="L63" t="s">
+        <v>90</v>
+      </c>
+      <c r="N63" t="s">
         <v>146</v>
       </c>
-      <c r="L63" t="s">
-        <v>90</v>
-      </c>
-      <c r="N63" t="s">
-        <v>147</v>
-      </c>
       <c r="O63" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B64" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" t="s">
         <v>130</v>
-      </c>
-      <c r="C64" t="s">
-        <v>131</v>
       </c>
       <c r="D64">
         <v>192.95</v>
@@ -4437,27 +4434,27 @@
         <v>16</v>
       </c>
       <c r="K64" t="s">
+        <v>145</v>
+      </c>
+      <c r="L64" t="s">
+        <v>90</v>
+      </c>
+      <c r="N64" t="s">
         <v>146</v>
       </c>
-      <c r="L64" t="s">
-        <v>90</v>
-      </c>
-      <c r="N64" t="s">
-        <v>147</v>
-      </c>
       <c r="O64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B65" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" t="s">
         <v>132</v>
-      </c>
-      <c r="C65" t="s">
-        <v>133</v>
       </c>
       <c r="D65">
         <v>350.07</v>
@@ -4478,27 +4475,27 @@
         <v>16</v>
       </c>
       <c r="K65" t="s">
+        <v>145</v>
+      </c>
+      <c r="L65" t="s">
+        <v>90</v>
+      </c>
+      <c r="N65" t="s">
         <v>146</v>
       </c>
-      <c r="L65" t="s">
-        <v>90</v>
-      </c>
-      <c r="N65" t="s">
-        <v>147</v>
-      </c>
       <c r="O65" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B66" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" t="s">
         <v>134</v>
-      </c>
-      <c r="C66" t="s">
-        <v>135</v>
       </c>
       <c r="D66">
         <v>232.36</v>
@@ -4519,27 +4516,27 @@
         <v>16</v>
       </c>
       <c r="K66" t="s">
+        <v>145</v>
+      </c>
+      <c r="L66" t="s">
+        <v>90</v>
+      </c>
+      <c r="N66" t="s">
         <v>146</v>
       </c>
-      <c r="L66" t="s">
-        <v>90</v>
-      </c>
-      <c r="N66" t="s">
-        <v>147</v>
-      </c>
       <c r="O66" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B67" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C67" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D67">
         <v>238.01</v>
@@ -4560,27 +4557,27 @@
         <v>16</v>
       </c>
       <c r="K67" t="s">
+        <v>145</v>
+      </c>
+      <c r="L67" t="s">
+        <v>90</v>
+      </c>
+      <c r="N67" t="s">
         <v>146</v>
       </c>
-      <c r="L67" t="s">
-        <v>90</v>
-      </c>
-      <c r="N67" t="s">
-        <v>147</v>
-      </c>
       <c r="O67" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C68" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D68">
         <v>172.1</v>
@@ -4601,27 +4598,27 @@
         <v>16</v>
       </c>
       <c r="K68" t="s">
+        <v>145</v>
+      </c>
+      <c r="L68" t="s">
+        <v>90</v>
+      </c>
+      <c r="N68" t="s">
         <v>146</v>
       </c>
-      <c r="L68" t="s">
-        <v>90</v>
-      </c>
-      <c r="N68" t="s">
-        <v>147</v>
-      </c>
       <c r="O68" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C69" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D69">
         <v>308.5</v>
@@ -4642,27 +4639,27 @@
         <v>16</v>
       </c>
       <c r="K69" t="s">
+        <v>145</v>
+      </c>
+      <c r="L69" t="s">
+        <v>90</v>
+      </c>
+      <c r="N69" t="s">
         <v>146</v>
       </c>
-      <c r="L69" t="s">
-        <v>90</v>
-      </c>
-      <c r="N69" t="s">
-        <v>147</v>
-      </c>
       <c r="O69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B70" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C70" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D70">
         <v>238.81</v>
@@ -4683,27 +4680,27 @@
         <v>16</v>
       </c>
       <c r="K70" t="s">
+        <v>145</v>
+      </c>
+      <c r="L70" t="s">
+        <v>90</v>
+      </c>
+      <c r="N70" t="s">
         <v>146</v>
       </c>
-      <c r="L70" t="s">
-        <v>90</v>
-      </c>
-      <c r="N70" t="s">
-        <v>147</v>
-      </c>
       <c r="O70" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B71" t="s">
+        <v>139</v>
+      </c>
+      <c r="C71" t="s">
         <v>140</v>
-      </c>
-      <c r="C71" t="s">
-        <v>141</v>
       </c>
       <c r="D71">
         <v>101.08</v>
@@ -4724,27 +4721,27 @@
         <v>16</v>
       </c>
       <c r="K71" t="s">
+        <v>145</v>
+      </c>
+      <c r="L71" t="s">
+        <v>90</v>
+      </c>
+      <c r="N71" t="s">
         <v>146</v>
       </c>
-      <c r="L71" t="s">
-        <v>90</v>
-      </c>
-      <c r="N71" t="s">
-        <v>147</v>
-      </c>
       <c r="O71" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B72" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C72" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D72">
         <v>170.89</v>
@@ -4765,27 +4762,27 @@
         <v>16</v>
       </c>
       <c r="K72" t="s">
+        <v>145</v>
+      </c>
+      <c r="L72" t="s">
+        <v>90</v>
+      </c>
+      <c r="N72" t="s">
         <v>146</v>
       </c>
-      <c r="L72" t="s">
-        <v>90</v>
-      </c>
-      <c r="N72" t="s">
-        <v>147</v>
-      </c>
       <c r="O72" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B73" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C73" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D73">
         <v>237.97</v>
@@ -4806,27 +4803,27 @@
         <v>16</v>
       </c>
       <c r="K73" t="s">
+        <v>145</v>
+      </c>
+      <c r="L73" t="s">
+        <v>90</v>
+      </c>
+      <c r="N73" t="s">
         <v>146</v>
       </c>
-      <c r="L73" t="s">
-        <v>90</v>
-      </c>
-      <c r="N73" t="s">
-        <v>147</v>
-      </c>
       <c r="O73" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B74" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C74" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D74">
         <v>237.57</v>
@@ -4847,27 +4844,27 @@
         <v>16</v>
       </c>
       <c r="K74" t="s">
+        <v>145</v>
+      </c>
+      <c r="L74" t="s">
+        <v>90</v>
+      </c>
+      <c r="N74" t="s">
         <v>146</v>
       </c>
-      <c r="L74" t="s">
-        <v>90</v>
-      </c>
-      <c r="N74" t="s">
-        <v>147</v>
-      </c>
       <c r="O74" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B75" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C75" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D75">
         <v>318.95999999999998</v>
@@ -4888,16 +4885,16 @@
         <v>16</v>
       </c>
       <c r="K75" t="s">
+        <v>145</v>
+      </c>
+      <c r="L75" t="s">
+        <v>90</v>
+      </c>
+      <c r="N75" t="s">
         <v>146</v>
       </c>
-      <c r="L75" t="s">
-        <v>90</v>
-      </c>
-      <c r="N75" t="s">
-        <v>147</v>
-      </c>
       <c r="O75" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
@@ -4941,10 +4938,10 @@
         <v>30</v>
       </c>
       <c r="N76" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O76" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
@@ -4955,7 +4952,7 @@
         <v>43</v>
       </c>
       <c r="C77" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D77">
         <v>511.6</v>
@@ -4988,10 +4985,10 @@
         <v>30</v>
       </c>
       <c r="N77" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O77" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
@@ -5002,7 +4999,7 @@
         <v>43</v>
       </c>
       <c r="C78" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D78">
         <v>442.2</v>
@@ -5035,10 +5032,10 @@
         <v>30</v>
       </c>
       <c r="N78" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O78" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
@@ -5049,7 +5046,7 @@
         <v>17</v>
       </c>
       <c r="C79" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D79">
         <v>34</v>
@@ -5073,21 +5070,21 @@
         <v>31</v>
       </c>
       <c r="N79" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O79" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B80" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C80" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D80">
         <v>38</v>
@@ -5117,24 +5114,24 @@
         <v>90</v>
       </c>
       <c r="M80" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N80" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O80" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B81" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C81" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D81">
         <v>33.299999999999997</v>
@@ -5164,24 +5161,24 @@
         <v>90</v>
       </c>
       <c r="M81" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N81" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O81" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B82" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C82" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D82">
         <v>31.62</v>
@@ -5211,13 +5208,13 @@
         <v>90</v>
       </c>
       <c r="M82" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N82" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O82" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
@@ -5261,21 +5258,21 @@
         <v>49</v>
       </c>
       <c r="N83" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O83" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B84" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C84" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D84">
         <v>118.8</v>
@@ -5293,30 +5290,30 @@
         <v>16</v>
       </c>
       <c r="K84" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L84" t="s">
         <v>90</v>
       </c>
       <c r="M84" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N84" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O84" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B85" t="s">
+        <v>163</v>
+      </c>
+      <c r="C85" t="s">
         <v>164</v>
-      </c>
-      <c r="C85" t="s">
-        <v>165</v>
       </c>
       <c r="D85">
         <v>103.8</v>
@@ -5334,30 +5331,30 @@
         <v>16</v>
       </c>
       <c r="K85" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L85" t="s">
         <v>90</v>
       </c>
       <c r="M85" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N85" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O85" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B86" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C86" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D86">
         <v>93.6</v>
@@ -5375,30 +5372,30 @@
         <v>16</v>
       </c>
       <c r="K86" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L86" t="s">
         <v>90</v>
       </c>
       <c r="M86" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N86" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O86" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B87" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C87" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D87">
         <v>111.5</v>
@@ -5416,30 +5413,30 @@
         <v>16</v>
       </c>
       <c r="K87" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L87" t="s">
         <v>90</v>
       </c>
       <c r="M87" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N87" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O87" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B88" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C88" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D88">
         <v>84.7</v>
@@ -5457,30 +5454,30 @@
         <v>16</v>
       </c>
       <c r="K88" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L88" t="s">
         <v>90</v>
       </c>
       <c r="M88" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N88" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O88" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B89" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C89" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D89">
         <v>97.2</v>
@@ -5498,30 +5495,30 @@
         <v>16</v>
       </c>
       <c r="K89" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L89" t="s">
         <v>90</v>
       </c>
       <c r="M89" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N89" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O89" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B90" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C90" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D90">
         <v>107.3</v>
@@ -5539,30 +5536,30 @@
         <v>16</v>
       </c>
       <c r="K90" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L90" t="s">
         <v>90</v>
       </c>
       <c r="M90" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N90" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O90" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B91" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C91" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D91">
         <v>53.2</v>
@@ -5592,21 +5589,21 @@
         <v>31</v>
       </c>
       <c r="N91" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O91" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B92" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C92" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D92">
         <v>34.4</v>
@@ -5636,21 +5633,21 @@
         <v>31</v>
       </c>
       <c r="N92" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O92" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B93" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C93" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D93">
         <v>32.700000000000003</v>
@@ -5680,21 +5677,21 @@
         <v>31</v>
       </c>
       <c r="N93" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O93" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B94" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C94" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D94">
         <v>53.5</v>
@@ -5724,21 +5721,21 @@
         <v>31</v>
       </c>
       <c r="N94" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O94" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>222</v>
+      </c>
+      <c r="B95" t="s">
         <v>125</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>126</v>
-      </c>
-      <c r="C95" t="s">
-        <v>127</v>
       </c>
       <c r="D95">
         <v>1047</v>
@@ -5768,24 +5765,24 @@
         <v>94</v>
       </c>
       <c r="M95" t="s">
+        <v>179</v>
+      </c>
+      <c r="N95" t="s">
         <v>180</v>
       </c>
-      <c r="N95" t="s">
-        <v>181</v>
-      </c>
       <c r="O95" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>222</v>
+      </c>
+      <c r="B96" t="s">
         <v>125</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
         <v>126</v>
-      </c>
-      <c r="C96" t="s">
-        <v>127</v>
       </c>
       <c r="D96">
         <v>1145</v>
@@ -5815,13 +5812,13 @@
         <v>93</v>
       </c>
       <c r="M96" t="s">
+        <v>179</v>
+      </c>
+      <c r="N96" t="s">
         <v>180</v>
       </c>
-      <c r="N96" t="s">
-        <v>181</v>
-      </c>
       <c r="O96" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
@@ -5850,19 +5847,19 @@
         <v>16</v>
       </c>
       <c r="K97" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L97" t="s">
         <v>90</v>
       </c>
       <c r="M97" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N97" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O97" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
@@ -5891,30 +5888,30 @@
         <v>16</v>
       </c>
       <c r="K98" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L98" t="s">
         <v>90</v>
       </c>
       <c r="M98" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N98" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O98" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B99" t="s">
+        <v>129</v>
+      </c>
+      <c r="C99" t="s">
         <v>130</v>
-      </c>
-      <c r="C99" t="s">
-        <v>131</v>
       </c>
       <c r="D99">
         <v>192.61</v>
@@ -5932,30 +5929,30 @@
         <v>16</v>
       </c>
       <c r="K99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L99" t="s">
         <v>90</v>
       </c>
       <c r="M99" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N99" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O99" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B100" t="s">
+        <v>129</v>
+      </c>
+      <c r="C100" t="s">
         <v>130</v>
-      </c>
-      <c r="C100" t="s">
-        <v>131</v>
       </c>
       <c r="D100">
         <v>158.21</v>
@@ -5973,30 +5970,30 @@
         <v>16</v>
       </c>
       <c r="K100" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L100" t="s">
         <v>90</v>
       </c>
       <c r="M100" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N100" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O100" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B101" t="s">
+        <v>133</v>
+      </c>
+      <c r="C101" t="s">
         <v>134</v>
-      </c>
-      <c r="C101" t="s">
-        <v>135</v>
       </c>
       <c r="D101">
         <v>255.43</v>
@@ -6014,30 +6011,30 @@
         <v>16</v>
       </c>
       <c r="K101" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L101" t="s">
         <v>90</v>
       </c>
       <c r="M101" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N101" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O101" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B102" t="s">
+        <v>133</v>
+      </c>
+      <c r="C102" t="s">
         <v>134</v>
-      </c>
-      <c r="C102" t="s">
-        <v>135</v>
       </c>
       <c r="D102">
         <v>195.92</v>
@@ -6055,30 +6052,30 @@
         <v>16</v>
       </c>
       <c r="K102" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L102" t="s">
         <v>90</v>
       </c>
       <c r="M102" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N102" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O102" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B103" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C103" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D103">
         <v>238.36</v>
@@ -6096,30 +6093,30 @@
         <v>16</v>
       </c>
       <c r="K103" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L103" t="s">
         <v>90</v>
       </c>
       <c r="M103" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N103" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O103" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B104" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C104" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D104">
         <v>177.29</v>
@@ -6137,30 +6134,30 @@
         <v>16</v>
       </c>
       <c r="K104" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L104" t="s">
         <v>90</v>
       </c>
       <c r="M104" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N104" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O104" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>184</v>
+      </c>
+      <c r="B105" t="s">
         <v>185</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>186</v>
-      </c>
-      <c r="C105" t="s">
-        <v>187</v>
       </c>
       <c r="D105">
         <v>108.6</v>
@@ -6187,24 +6184,24 @@
         <v>90</v>
       </c>
       <c r="M105" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N105" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O105" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>184</v>
+      </c>
+      <c r="B106" t="s">
         <v>185</v>
       </c>
-      <c r="B106" t="s">
-        <v>186</v>
-      </c>
       <c r="C106" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D106">
         <v>90.7</v>
@@ -6231,24 +6228,24 @@
         <v>90</v>
       </c>
       <c r="M106" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N106" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O106" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>184</v>
+      </c>
+      <c r="B107" t="s">
         <v>185</v>
       </c>
-      <c r="B107" t="s">
-        <v>186</v>
-      </c>
       <c r="C107" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D107">
         <v>106.9</v>
@@ -6275,24 +6272,24 @@
         <v>90</v>
       </c>
       <c r="M107" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N107" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O107" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>184</v>
+      </c>
+      <c r="B108" t="s">
         <v>185</v>
       </c>
-      <c r="B108" t="s">
-        <v>186</v>
-      </c>
       <c r="C108" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D108">
         <v>111.3</v>
@@ -6319,24 +6316,24 @@
         <v>90</v>
       </c>
       <c r="M108" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N108" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O108" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>192</v>
+      </c>
+      <c r="B109" t="s">
         <v>193</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>194</v>
-      </c>
-      <c r="C109" t="s">
-        <v>195</v>
       </c>
       <c r="D109">
         <v>897</v>
@@ -6360,7 +6357,7 @@
         <v>16</v>
       </c>
       <c r="K109" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L109" t="s">
         <v>90</v>
@@ -6369,21 +6366,21 @@
         <v>31</v>
       </c>
       <c r="N109" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O109" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>192</v>
+      </c>
+      <c r="B110" t="s">
         <v>193</v>
       </c>
-      <c r="B110" t="s">
-        <v>194</v>
-      </c>
       <c r="C110" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D110">
         <v>1838</v>
@@ -6407,7 +6404,7 @@
         <v>16</v>
       </c>
       <c r="K110" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L110" t="s">
         <v>90</v>
@@ -6416,10 +6413,10 @@
         <v>31</v>
       </c>
       <c r="N110" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
@@ -6463,10 +6460,10 @@
         <v>99</v>
       </c>
       <c r="N111" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O111" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
@@ -6510,10 +6507,10 @@
         <v>99</v>
       </c>
       <c r="N112" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O112" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
@@ -6524,7 +6521,7 @@
         <v>43</v>
       </c>
       <c r="C113" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D113">
         <v>326.28399999999999</v>
@@ -6557,10 +6554,10 @@
         <v>99</v>
       </c>
       <c r="N113" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O113" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
@@ -6571,7 +6568,7 @@
         <v>43</v>
       </c>
       <c r="C114" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D114">
         <v>281.81400000000002</v>
@@ -6604,10 +6601,10 @@
         <v>99</v>
       </c>
       <c r="N114" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O114" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
@@ -6618,7 +6615,7 @@
         <v>43</v>
       </c>
       <c r="C115" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D115">
         <v>326.59500000000003</v>
@@ -6651,10 +6648,10 @@
         <v>99</v>
       </c>
       <c r="N115" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O115" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
@@ -6665,7 +6662,7 @@
         <v>43</v>
       </c>
       <c r="C116" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D116">
         <v>638.68299999999999</v>
@@ -6698,10 +6695,10 @@
         <v>99</v>
       </c>
       <c r="N116" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O116" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
@@ -6712,7 +6709,7 @@
         <v>43</v>
       </c>
       <c r="C117" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D117">
         <v>787.18600000000004</v>
@@ -6745,10 +6742,10 @@
         <v>99</v>
       </c>
       <c r="N117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O117" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
@@ -6792,10 +6789,10 @@
         <v>99</v>
       </c>
       <c r="N118" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O118" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
@@ -6806,7 +6803,7 @@
         <v>76</v>
       </c>
       <c r="C119" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D119">
         <v>420.03300000000002</v>
@@ -6839,10 +6836,10 @@
         <v>99</v>
       </c>
       <c r="N119" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O119" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
@@ -6853,7 +6850,7 @@
         <v>76</v>
       </c>
       <c r="C120" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D120">
         <v>262.21600000000001</v>
@@ -6886,10 +6883,10 @@
         <v>99</v>
       </c>
       <c r="N120" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O120" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
@@ -6900,7 +6897,7 @@
         <v>76</v>
       </c>
       <c r="C121" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D121">
         <v>189.655</v>
@@ -6930,10 +6927,10 @@
         <v>99</v>
       </c>
       <c r="N121" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O121" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
@@ -6944,7 +6941,7 @@
         <v>76</v>
       </c>
       <c r="C122" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D122">
         <v>311.29399999999998</v>
@@ -6977,10 +6974,10 @@
         <v>99</v>
       </c>
       <c r="N122" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O122" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
@@ -7015,10 +7012,10 @@
         <v>99</v>
       </c>
       <c r="N123" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O123" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
@@ -7053,10 +7050,10 @@
         <v>99</v>
       </c>
       <c r="N124" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O124" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
@@ -7067,7 +7064,7 @@
         <v>108</v>
       </c>
       <c r="C125" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D125">
         <v>80</v>
@@ -7082,19 +7079,19 @@
         <v>16</v>
       </c>
       <c r="K125" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L125" t="s">
         <v>90</v>
       </c>
       <c r="M125" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N125" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O125" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
@@ -7105,7 +7102,7 @@
         <v>108</v>
       </c>
       <c r="C126" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D126">
         <v>78</v>
@@ -7120,19 +7117,19 @@
         <v>16</v>
       </c>
       <c r="K126" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L126" t="s">
         <v>90</v>
       </c>
       <c r="M126" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N126" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O126" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.25">
@@ -7143,7 +7140,7 @@
         <v>108</v>
       </c>
       <c r="C127" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D127">
         <v>89</v>
@@ -7158,19 +7155,19 @@
         <v>16</v>
       </c>
       <c r="K127" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L127" t="s">
         <v>90</v>
       </c>
       <c r="M127" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N127" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O127" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.25">
@@ -7181,7 +7178,7 @@
         <v>108</v>
       </c>
       <c r="C128" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D128">
         <v>78</v>
@@ -7196,19 +7193,19 @@
         <v>16</v>
       </c>
       <c r="K128" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L128" t="s">
         <v>90</v>
       </c>
       <c r="M128" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N128" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O128" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.25">
@@ -7219,7 +7216,7 @@
         <v>108</v>
       </c>
       <c r="C129" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D129">
         <v>84</v>
@@ -7234,19 +7231,19 @@
         <v>16</v>
       </c>
       <c r="K129" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L129" t="s">
         <v>90</v>
       </c>
       <c r="M129" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N129" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O129" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.25">
@@ -7257,7 +7254,7 @@
         <v>108</v>
       </c>
       <c r="C130" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D130">
         <v>78</v>
@@ -7272,19 +7269,19 @@
         <v>16</v>
       </c>
       <c r="K130" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L130" t="s">
         <v>90</v>
       </c>
       <c r="M130" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N130" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O130" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.25">
@@ -7310,19 +7307,19 @@
         <v>16</v>
       </c>
       <c r="K131" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L131" t="s">
         <v>90</v>
       </c>
       <c r="M131" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N131" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O131" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.25">
@@ -7348,19 +7345,19 @@
         <v>16</v>
       </c>
       <c r="K132" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L132" t="s">
         <v>90</v>
       </c>
       <c r="M132" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N132" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O132" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.25">
@@ -7386,19 +7383,19 @@
         <v>16</v>
       </c>
       <c r="K133" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L133" t="s">
         <v>90</v>
       </c>
       <c r="M133" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N133" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O133" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.25">
@@ -7424,19 +7421,19 @@
         <v>16</v>
       </c>
       <c r="K134" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L134" t="s">
         <v>90</v>
       </c>
       <c r="M134" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N134" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O134" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.25">
@@ -7462,19 +7459,19 @@
         <v>16</v>
       </c>
       <c r="K135" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L135" t="s">
         <v>90</v>
       </c>
       <c r="M135" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N135" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O135" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.25">
@@ -7500,30 +7497,30 @@
         <v>16</v>
       </c>
       <c r="K136" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L136" t="s">
         <v>90</v>
       </c>
       <c r="M136" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N136" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O136" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B137" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C137" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D137">
         <v>157</v>
@@ -7538,30 +7535,30 @@
         <v>16</v>
       </c>
       <c r="K137" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L137" t="s">
         <v>90</v>
       </c>
       <c r="M137" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N137" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O137" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B138" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C138" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D138">
         <v>135</v>
@@ -7576,30 +7573,30 @@
         <v>16</v>
       </c>
       <c r="K138" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L138" t="s">
         <v>90</v>
       </c>
       <c r="M138" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N138" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O138" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B139" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C139" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D139">
         <v>173</v>
@@ -7614,30 +7611,30 @@
         <v>16</v>
       </c>
       <c r="K139" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L139" t="s">
         <v>90</v>
       </c>
       <c r="M139" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N139" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O139" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B140" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C140" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D140">
         <v>135</v>
@@ -7652,30 +7649,30 @@
         <v>16</v>
       </c>
       <c r="K140" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L140" t="s">
         <v>90</v>
       </c>
       <c r="M140" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N140" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O140" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B141" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C141" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D141">
         <v>135</v>
@@ -7690,19 +7687,19 @@
         <v>16</v>
       </c>
       <c r="K141" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L141" t="s">
         <v>90</v>
       </c>
       <c r="M141" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N141" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O141" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.25">
@@ -7731,19 +7728,19 @@
         <v>16</v>
       </c>
       <c r="K142" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L142" t="s">
         <v>90</v>
       </c>
       <c r="M142" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N142" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O142" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.25">
@@ -7784,24 +7781,24 @@
         <v>90</v>
       </c>
       <c r="M143" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N143" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O143" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>222</v>
+      </c>
+      <c r="B144" t="s">
         <v>223</v>
       </c>
-      <c r="B144" t="s">
+      <c r="C144" t="s">
         <v>224</v>
-      </c>
-      <c r="C144" t="s">
-        <v>225</v>
       </c>
       <c r="D144">
         <v>198.94</v>
@@ -7825,19 +7822,19 @@
         <v>16</v>
       </c>
       <c r="K144" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L144" t="s">
         <v>90</v>
       </c>
       <c r="M144" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N144" t="s">
+        <v>218</v>
+      </c>
+      <c r="O144" t="s">
         <v>219</v>
-      </c>
-      <c r="O144" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.25">
@@ -7869,19 +7866,19 @@
         <v>36</v>
       </c>
       <c r="K145" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L145" t="s">
         <v>90</v>
       </c>
       <c r="M145" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N145" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O145" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="146" spans="1:15" x14ac:dyDescent="0.25">
@@ -7922,24 +7919,24 @@
         <v>90</v>
       </c>
       <c r="M146" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N146" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O146" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B147" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C147" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D147">
         <v>46.8</v>
@@ -7960,30 +7957,30 @@
         <v>36</v>
       </c>
       <c r="K147" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L147" t="s">
         <v>90</v>
       </c>
       <c r="M147" t="s">
+        <v>228</v>
+      </c>
+      <c r="N147" t="s">
         <v>229</v>
       </c>
-      <c r="N147" t="s">
-        <v>230</v>
-      </c>
       <c r="O147" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B148" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C148" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D148">
         <v>42.9</v>
@@ -8004,30 +8001,30 @@
         <v>36</v>
       </c>
       <c r="K148" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L148" t="s">
         <v>90</v>
       </c>
       <c r="M148" t="s">
+        <v>228</v>
+      </c>
+      <c r="N148" t="s">
         <v>229</v>
       </c>
-      <c r="N148" t="s">
-        <v>230</v>
-      </c>
       <c r="O148" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B149" t="s">
+        <v>129</v>
+      </c>
+      <c r="C149" t="s">
         <v>130</v>
-      </c>
-      <c r="C149" t="s">
-        <v>131</v>
       </c>
       <c r="D149">
         <v>25.6</v>
@@ -8045,30 +8042,30 @@
         <v>36</v>
       </c>
       <c r="K149" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L149" t="s">
         <v>90</v>
       </c>
       <c r="M149" t="s">
+        <v>228</v>
+      </c>
+      <c r="N149" t="s">
         <v>229</v>
       </c>
-      <c r="N149" t="s">
-        <v>230</v>
-      </c>
       <c r="O149" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B150" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C150" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D150">
         <v>21.7</v>
@@ -8086,19 +8083,19 @@
         <v>36</v>
       </c>
       <c r="K150" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L150" t="s">
         <v>90</v>
       </c>
       <c r="M150" t="s">
+        <v>228</v>
+      </c>
+      <c r="N150" t="s">
         <v>229</v>
       </c>
-      <c r="N150" t="s">
-        <v>230</v>
-      </c>
       <c r="O150" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.25">
@@ -8109,7 +8106,7 @@
         <v>43</v>
       </c>
       <c r="C151" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D151">
         <v>282.13</v>
@@ -8139,10 +8136,10 @@
         <v>99</v>
       </c>
       <c r="N151" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O151" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="152" spans="1:15" x14ac:dyDescent="0.25">
@@ -8153,7 +8150,7 @@
         <v>43</v>
       </c>
       <c r="C152" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D152">
         <v>274.60000000000002</v>
@@ -8180,13 +8177,13 @@
         <v>90</v>
       </c>
       <c r="M152" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N152" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O152" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="153" spans="1:15" x14ac:dyDescent="0.25">
@@ -8227,10 +8224,10 @@
         <v>99</v>
       </c>
       <c r="N153" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O153" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="154" spans="1:15" x14ac:dyDescent="0.25">
@@ -8268,13 +8265,13 @@
         <v>90</v>
       </c>
       <c r="M154" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N154" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O154" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="155" spans="1:15" x14ac:dyDescent="0.25">
@@ -8315,10 +8312,10 @@
         <v>99</v>
       </c>
       <c r="N155" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O155" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="156" spans="1:15" x14ac:dyDescent="0.25">
@@ -8356,13 +8353,13 @@
         <v>90</v>
       </c>
       <c r="M156" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N156" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O156" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="157" spans="1:15" x14ac:dyDescent="0.25">
@@ -8373,7 +8370,7 @@
         <v>17</v>
       </c>
       <c r="C157" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D157">
         <v>296</v>
@@ -8400,24 +8397,24 @@
         <v>90</v>
       </c>
       <c r="M157" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N157" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O157" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B158" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C158" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D158">
         <v>308</v>
@@ -8444,13 +8441,13 @@
         <v>90</v>
       </c>
       <c r="M158" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N158" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O158" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="159" spans="1:15" x14ac:dyDescent="0.25">
@@ -8488,13 +8485,13 @@
         <v>90</v>
       </c>
       <c r="M159" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N159" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O159" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="160" spans="1:15" x14ac:dyDescent="0.25">
@@ -8532,24 +8529,24 @@
         <v>90</v>
       </c>
       <c r="M160" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N160" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O160" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B161" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C161" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D161">
         <v>263</v>
@@ -8579,24 +8576,24 @@
         <v>90</v>
       </c>
       <c r="M161" t="s">
+        <v>238</v>
+      </c>
+      <c r="N161" t="s">
         <v>239</v>
       </c>
-      <c r="N161" t="s">
-        <v>240</v>
-      </c>
       <c r="O161" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B162" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C162" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D162">
         <v>402</v>
@@ -8626,24 +8623,24 @@
         <v>90</v>
       </c>
       <c r="M162" t="s">
+        <v>238</v>
+      </c>
+      <c r="N162" t="s">
         <v>239</v>
       </c>
-      <c r="N162" t="s">
-        <v>240</v>
-      </c>
       <c r="O162" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B163" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C163" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D163">
         <v>372</v>
@@ -8673,24 +8670,24 @@
         <v>90</v>
       </c>
       <c r="M163" t="s">
+        <v>238</v>
+      </c>
+      <c r="N163" t="s">
         <v>239</v>
       </c>
-      <c r="N163" t="s">
-        <v>240</v>
-      </c>
       <c r="O163" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B164" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C164" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D164">
         <v>457</v>
@@ -8720,24 +8717,24 @@
         <v>90</v>
       </c>
       <c r="M164" t="s">
+        <v>238</v>
+      </c>
+      <c r="N164" t="s">
         <v>239</v>
       </c>
-      <c r="N164" t="s">
-        <v>240</v>
-      </c>
       <c r="O164" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B165" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C165" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D165">
         <v>218</v>
@@ -8767,24 +8764,24 @@
         <v>90</v>
       </c>
       <c r="M165" t="s">
+        <v>238</v>
+      </c>
+      <c r="N165" t="s">
         <v>239</v>
       </c>
-      <c r="N165" t="s">
-        <v>240</v>
-      </c>
       <c r="O165" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B166" t="s">
+        <v>131</v>
+      </c>
+      <c r="C166" t="s">
         <v>132</v>
-      </c>
-      <c r="C166" t="s">
-        <v>133</v>
       </c>
       <c r="D166">
         <v>366</v>
@@ -8814,24 +8811,24 @@
         <v>90</v>
       </c>
       <c r="M166" t="s">
+        <v>238</v>
+      </c>
+      <c r="N166" t="s">
         <v>239</v>
       </c>
-      <c r="N166" t="s">
-        <v>240</v>
-      </c>
       <c r="O166" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B167" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C167" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D167">
         <v>339</v>
@@ -8861,24 +8858,24 @@
         <v>90</v>
       </c>
       <c r="M167" t="s">
+        <v>238</v>
+      </c>
+      <c r="N167" t="s">
         <v>239</v>
       </c>
-      <c r="N167" t="s">
-        <v>240</v>
-      </c>
       <c r="O167" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B168" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C168" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D168">
         <v>281</v>
@@ -8908,24 +8905,24 @@
         <v>90</v>
       </c>
       <c r="M168" t="s">
+        <v>238</v>
+      </c>
+      <c r="N168" t="s">
         <v>239</v>
       </c>
-      <c r="N168" t="s">
-        <v>240</v>
-      </c>
       <c r="O168" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B169" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C169" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D169">
         <v>310</v>
@@ -8955,24 +8952,24 @@
         <v>90</v>
       </c>
       <c r="M169" t="s">
+        <v>238</v>
+      </c>
+      <c r="N169" t="s">
         <v>239</v>
       </c>
-      <c r="N169" t="s">
-        <v>240</v>
-      </c>
       <c r="O169" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="170" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B170" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C170" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D170">
         <v>207</v>
@@ -9002,24 +8999,24 @@
         <v>90</v>
       </c>
       <c r="M170" t="s">
+        <v>238</v>
+      </c>
+      <c r="N170" t="s">
         <v>239</v>
       </c>
-      <c r="N170" t="s">
-        <v>240</v>
-      </c>
       <c r="O170" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B171" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C171" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D171">
         <v>376</v>
@@ -9049,24 +9046,24 @@
         <v>90</v>
       </c>
       <c r="M171" t="s">
+        <v>238</v>
+      </c>
+      <c r="N171" t="s">
         <v>239</v>
       </c>
-      <c r="N171" t="s">
-        <v>240</v>
-      </c>
       <c r="O171" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="172" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B172" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C172" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D172">
         <v>252</v>
@@ -9096,24 +9093,24 @@
         <v>90</v>
       </c>
       <c r="M172" t="s">
+        <v>238</v>
+      </c>
+      <c r="N172" t="s">
         <v>239</v>
       </c>
-      <c r="N172" t="s">
-        <v>240</v>
-      </c>
       <c r="O172" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="173" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>184</v>
+      </c>
+      <c r="B173" t="s">
         <v>185</v>
       </c>
-      <c r="B173" t="s">
-        <v>186</v>
-      </c>
       <c r="C173" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D173">
         <v>11</v>
@@ -9143,24 +9140,24 @@
         <v>90</v>
       </c>
       <c r="M173" t="s">
+        <v>248</v>
+      </c>
+      <c r="N173" t="s">
         <v>249</v>
       </c>
-      <c r="N173" t="s">
-        <v>250</v>
-      </c>
       <c r="O173" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="174" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="B174" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C174" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D174">
         <v>47.38</v>
@@ -9190,13 +9187,13 @@
         <v>90</v>
       </c>
       <c r="M174" t="s">
+        <v>248</v>
+      </c>
+      <c r="N174" t="s">
         <v>249</v>
       </c>
-      <c r="N174" t="s">
-        <v>250</v>
-      </c>
       <c r="O174" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="175" spans="1:15" x14ac:dyDescent="0.25">
@@ -9237,13 +9234,13 @@
         <v>90</v>
       </c>
       <c r="M175" t="s">
+        <v>248</v>
+      </c>
+      <c r="N175" t="s">
         <v>249</v>
       </c>
-      <c r="N175" t="s">
-        <v>250</v>
-      </c>
       <c r="O175" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="176" spans="1:15" x14ac:dyDescent="0.25">
@@ -9284,13 +9281,13 @@
         <v>90</v>
       </c>
       <c r="M176" t="s">
+        <v>248</v>
+      </c>
+      <c r="N176" t="s">
         <v>249</v>
       </c>
-      <c r="N176" t="s">
-        <v>250</v>
-      </c>
       <c r="O176" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.25">
@@ -9331,13 +9328,13 @@
         <v>93</v>
       </c>
       <c r="M177" t="s">
+        <v>248</v>
+      </c>
+      <c r="N177" t="s">
         <v>249</v>
       </c>
-      <c r="N177" t="s">
-        <v>250</v>
-      </c>
       <c r="O177" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.25">
@@ -9378,13 +9375,13 @@
         <v>94</v>
       </c>
       <c r="M178" t="s">
+        <v>248</v>
+      </c>
+      <c r="N178" t="s">
         <v>249</v>
       </c>
-      <c r="N178" t="s">
-        <v>250</v>
-      </c>
       <c r="O178" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.25">
@@ -9395,7 +9392,7 @@
         <v>17</v>
       </c>
       <c r="C179" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D179">
         <v>22.37</v>
@@ -9425,13 +9422,13 @@
         <v>93</v>
       </c>
       <c r="M179" t="s">
+        <v>248</v>
+      </c>
+      <c r="N179" t="s">
         <v>249</v>
       </c>
-      <c r="N179" t="s">
-        <v>250</v>
-      </c>
       <c r="O179" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.25">
@@ -9442,7 +9439,7 @@
         <v>17</v>
       </c>
       <c r="C180" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D180">
         <v>19.75</v>
@@ -9472,13 +9469,13 @@
         <v>94</v>
       </c>
       <c r="M180" t="s">
+        <v>248</v>
+      </c>
+      <c r="N180" t="s">
         <v>249</v>
       </c>
-      <c r="N180" t="s">
-        <v>250</v>
-      </c>
       <c r="O180" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.25">
@@ -9519,13 +9516,13 @@
         <v>93</v>
       </c>
       <c r="M181" t="s">
+        <v>248</v>
+      </c>
+      <c r="N181" t="s">
         <v>249</v>
       </c>
-      <c r="N181" t="s">
-        <v>250</v>
-      </c>
       <c r="O181" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.25">
@@ -9566,24 +9563,24 @@
         <v>94</v>
       </c>
       <c r="M182" t="s">
+        <v>248</v>
+      </c>
+      <c r="N182" t="s">
         <v>249</v>
       </c>
-      <c r="N182" t="s">
-        <v>250</v>
-      </c>
       <c r="O182" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="183" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
+        <v>184</v>
+      </c>
+      <c r="B183" t="s">
         <v>185</v>
       </c>
-      <c r="B183" t="s">
-        <v>186</v>
-      </c>
       <c r="C183" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D183">
         <v>10.99</v>
@@ -9613,13 +9610,13 @@
         <v>90</v>
       </c>
       <c r="M183" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N183" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O183" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="184" spans="1:15" x14ac:dyDescent="0.25">
@@ -9660,13 +9657,13 @@
         <v>90</v>
       </c>
       <c r="M184" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N184" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O184" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="185" spans="1:15" x14ac:dyDescent="0.25">
@@ -9707,13 +9704,13 @@
         <v>93</v>
       </c>
       <c r="M185" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N185" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O185" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="186" spans="1:15" x14ac:dyDescent="0.25">
@@ -9754,13 +9751,13 @@
         <v>94</v>
       </c>
       <c r="M186" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N186" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O186" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.25">
@@ -9801,13 +9798,13 @@
         <v>93</v>
       </c>
       <c r="M187" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N187" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O187" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="188" spans="1:15" x14ac:dyDescent="0.25">
@@ -9848,24 +9845,24 @@
         <v>94</v>
       </c>
       <c r="M188" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N188" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O188" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="189" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
+        <v>184</v>
+      </c>
+      <c r="B189" t="s">
         <v>185</v>
       </c>
-      <c r="B189" t="s">
-        <v>186</v>
-      </c>
       <c r="C189" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D189">
         <v>10.7</v>
@@ -9895,13 +9892,13 @@
         <v>90</v>
       </c>
       <c r="M189" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N189" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O189" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.25">
@@ -9942,13 +9939,13 @@
         <v>90</v>
       </c>
       <c r="M190" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N190" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O190" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="191" spans="1:15" x14ac:dyDescent="0.25">
@@ -9989,13 +9986,13 @@
         <v>93</v>
       </c>
       <c r="M191" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N191" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O191" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="192" spans="1:15" x14ac:dyDescent="0.25">
@@ -10036,13 +10033,13 @@
         <v>94</v>
       </c>
       <c r="M192" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N192" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O192" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="193" spans="1:15" x14ac:dyDescent="0.25">
@@ -10083,13 +10080,13 @@
         <v>93</v>
       </c>
       <c r="M193" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N193" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O193" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.25">
@@ -10130,13 +10127,13 @@
         <v>94</v>
       </c>
       <c r="M194" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N194" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O194" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="195" spans="1:15" x14ac:dyDescent="0.25">
@@ -10177,24 +10174,24 @@
         <v>90</v>
       </c>
       <c r="M195" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N195" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O195" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="196" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
+        <v>184</v>
+      </c>
+      <c r="B196" t="s">
         <v>185</v>
       </c>
-      <c r="B196" t="s">
-        <v>186</v>
-      </c>
       <c r="C196" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D196">
         <v>10.52</v>
@@ -10224,13 +10221,13 @@
         <v>90</v>
       </c>
       <c r="M196" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N196" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O196" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="197" spans="1:15" x14ac:dyDescent="0.25">
@@ -10271,13 +10268,13 @@
         <v>90</v>
       </c>
       <c r="M197" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N197" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O197" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="198" spans="1:15" x14ac:dyDescent="0.25">
@@ -10318,13 +10315,13 @@
         <v>93</v>
       </c>
       <c r="M198" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N198" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O198" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="199" spans="1:15" x14ac:dyDescent="0.25">
@@ -10365,13 +10362,13 @@
         <v>94</v>
       </c>
       <c r="M199" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N199" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O199" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="200" spans="1:15" x14ac:dyDescent="0.25">
@@ -10412,13 +10409,13 @@
         <v>93</v>
       </c>
       <c r="M200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N200" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O200" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="201" spans="1:15" x14ac:dyDescent="0.25">
@@ -10459,13 +10456,13 @@
         <v>94</v>
       </c>
       <c r="M201" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N201" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O201" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="202" spans="1:15" x14ac:dyDescent="0.25">
@@ -10506,13 +10503,13 @@
         <v>93</v>
       </c>
       <c r="M202" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N202" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O202" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="203" spans="1:15" x14ac:dyDescent="0.25">
@@ -10553,13 +10550,13 @@
         <v>94</v>
       </c>
       <c r="M203" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N203" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O203" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -10703,10 +10700,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>